<commit_message>
Add Batch ID Column to Batch Header Sheet and reorder assignment commands
</commit_message>
<xml_diff>
--- a/CASH REPORT.xlsx
+++ b/CASH REPORT.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FW5"/>
+  <dimension ref="A1:FX5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,890 +442,895 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>BATCHID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>ENTRYNO</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>ENTRYTYPE</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>REFERENCE</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>PERIOD</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>DATE</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>DATECHQPRN</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>SWCHQPRN</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>MISCCODE</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>TEXTDESC</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>DISTCODE</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>CHARGECODE</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>CHRGAMOUNT</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>NODETAILS</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>TOTAMOUNT</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>TOTTAX</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>TAXPERCNT</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>BK2GLCURHM</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>BK2GLRTTYP</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>BK2GLCURSR</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>BK2GLDATE</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>BK2GLRATE</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>BK2GLSPRD</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>BK2GLOP</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>BK2GLDTMTH</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>BT2GLCURHM</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>BT2GLRTTYP</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>BT2GLCURSR</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>BT2GLDATE</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>BT2GLRATE</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>BT2GLSPRD</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>BT2GLOP</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>BT2GLDTMTH</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>MS2GLCURHM</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>MS2GLRTTYP</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>MS2GLCURSR</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>MS2GLDATE</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>MS2GLRATE</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>MS2GLSPRD</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>MS2GLOP</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>MS2GLDTMTH</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>SWCASH</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>BTCHNODEC</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>MISCNODEC</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>TAXGROUP</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>CUSTCHQNO</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>NOSUBDETL</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>APPLAMOUNT</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>APPLDISC</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>ACCTNAT</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>ADJAMOUNT</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>PROFILEID</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>SWINTERCO</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>FISCYR</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>CCTYPE</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>CCNUMBER</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>CCNAME</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>CCEXP</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>CCAUTHCODE</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>XCCNUMBER</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>SERIAL</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>BANKAMOUNT</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>BTCHAMOUNT</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>MISCAMOUNT</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>FUNCAMOUNT</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>HDRDEBIT</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>HDRCREDIT</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>TAXAUTH1</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>TAXAUTH2</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>TAXAUTH3</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>TAXAUTH4</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>TAXAUTH5</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>TXAU1DESC</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>TXAU2DESC</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>TXAU3DESC</t>
         </is>
       </c>
-      <c r="BX1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
           <t>TXAU4DESC</t>
         </is>
       </c>
-      <c r="BY1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>TXAU5DESC</t>
         </is>
       </c>
-      <c r="BZ1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>TAXCLASS1</t>
         </is>
       </c>
-      <c r="CA1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>TAXCLASS2</t>
         </is>
       </c>
-      <c r="CB1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>TAXCLASS3</t>
         </is>
       </c>
-      <c r="CC1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>TAXCLASS4</t>
         </is>
       </c>
-      <c r="CD1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>TAXCLASS5</t>
         </is>
       </c>
-      <c r="CE1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>BASETAX1</t>
         </is>
       </c>
-      <c r="CF1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>BASETAX2</t>
         </is>
       </c>
-      <c r="CG1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>BASETAX3</t>
         </is>
       </c>
-      <c r="CH1" s="1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>BASETAX4</t>
         </is>
       </c>
-      <c r="CI1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>BASETAX5</t>
         </is>
       </c>
-      <c r="CJ1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>AMTTAX1</t>
         </is>
       </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>AMTTAX2</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>AMTTAX3</t>
         </is>
       </c>
-      <c r="CM1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>AMTTAX4</t>
         </is>
       </c>
-      <c r="CN1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>AMTTAX5</t>
         </is>
       </c>
-      <c r="CO1" s="1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>SWTAXINCL1</t>
         </is>
       </c>
-      <c r="CP1" s="1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>SWTAXINCL2</t>
         </is>
       </c>
-      <c r="CQ1" s="1" t="inlineStr">
+      <c r="CR1" s="1" t="inlineStr">
         <is>
           <t>SWTAXINCL3</t>
         </is>
       </c>
-      <c r="CR1" s="1" t="inlineStr">
+      <c r="CS1" s="1" t="inlineStr">
         <is>
           <t>SWTAXINCL4</t>
         </is>
       </c>
-      <c r="CS1" s="1" t="inlineStr">
+      <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>SWTAXINCL5</t>
         </is>
       </c>
-      <c r="CT1" s="1" t="inlineStr">
+      <c r="CU1" s="1" t="inlineStr">
         <is>
           <t>BANKCODE</t>
         </is>
       </c>
-      <c r="CU1" s="1" t="inlineStr">
+      <c r="CV1" s="1" t="inlineStr">
         <is>
           <t>SWPOSTED</t>
         </is>
       </c>
-      <c r="CV1" s="1" t="inlineStr">
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>VALUES</t>
         </is>
       </c>
-      <c r="CW1" s="1" t="inlineStr">
+      <c r="CX1" s="1" t="inlineStr">
         <is>
           <t>PROCESSCMD</t>
         </is>
       </c>
-      <c r="CX1" s="1" t="inlineStr">
+      <c r="CY1" s="1" t="inlineStr">
         <is>
           <t>TOTUNAPPL</t>
         </is>
       </c>
-      <c r="CY1" s="1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>TOTAPPLAMT</t>
         </is>
       </c>
-      <c r="CZ1" s="1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>TOTAPPLDSC</t>
         </is>
       </c>
-      <c r="DA1" s="1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>ALLOCMODE</t>
         </is>
       </c>
-      <c r="DB1" s="1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
         <is>
           <t>ALLOCAMT</t>
         </is>
       </c>
-      <c r="DC1" s="1" t="inlineStr">
+      <c r="DD1" s="1" t="inlineStr">
         <is>
           <t>CLASSTYPE</t>
         </is>
       </c>
-      <c r="DD1" s="1" t="inlineStr">
+      <c r="DE1" s="1" t="inlineStr">
         <is>
           <t>CLASSAXIS</t>
         </is>
       </c>
-      <c r="DE1" s="1" t="inlineStr">
+      <c r="DF1" s="1" t="inlineStr">
         <is>
           <t>DATALEVEL</t>
         </is>
       </c>
-      <c r="DF1" s="1" t="inlineStr">
+      <c r="DG1" s="1" t="inlineStr">
         <is>
           <t>RECXCNTER</t>
         </is>
       </c>
-      <c r="DG1" s="1" t="inlineStr">
+      <c r="DH1" s="1" t="inlineStr">
         <is>
           <t>RATERC</t>
         </is>
       </c>
-      <c r="DH1" s="1" t="inlineStr">
+      <c r="DI1" s="1" t="inlineStr">
         <is>
           <t>RATETYPERC</t>
         </is>
       </c>
-      <c r="DI1" s="1" t="inlineStr">
+      <c r="DJ1" s="1" t="inlineStr">
         <is>
           <t>RATEOPRC</t>
         </is>
       </c>
-      <c r="DJ1" s="1" t="inlineStr">
+      <c r="DK1" s="1" t="inlineStr">
         <is>
           <t>RATEDATERC</t>
         </is>
       </c>
-      <c r="DK1" s="1" t="inlineStr">
+      <c r="DL1" s="1" t="inlineStr">
         <is>
           <t>CODECURNRC</t>
         </is>
       </c>
-      <c r="DL1" s="1" t="inlineStr">
+      <c r="DM1" s="1" t="inlineStr">
         <is>
           <t>TXAMT1RC</t>
         </is>
       </c>
-      <c r="DM1" s="1" t="inlineStr">
+      <c r="DN1" s="1" t="inlineStr">
         <is>
           <t>TXAMT2RC</t>
         </is>
       </c>
-      <c r="DN1" s="1" t="inlineStr">
+      <c r="DO1" s="1" t="inlineStr">
         <is>
           <t>TXAMT3RC</t>
         </is>
       </c>
-      <c r="DO1" s="1" t="inlineStr">
+      <c r="DP1" s="1" t="inlineStr">
         <is>
           <t>TXAMT4RC</t>
         </is>
       </c>
-      <c r="DP1" s="1" t="inlineStr">
+      <c r="DQ1" s="1" t="inlineStr">
         <is>
           <t>TXAMT5RC</t>
         </is>
       </c>
-      <c r="DQ1" s="1" t="inlineStr">
+      <c r="DR1" s="1" t="inlineStr">
         <is>
           <t>TXTOTRC</t>
         </is>
       </c>
-      <c r="DR1" s="1" t="inlineStr">
+      <c r="DS1" s="1" t="inlineStr">
         <is>
           <t>TXALLRC</t>
         </is>
       </c>
-      <c r="DS1" s="1" t="inlineStr">
+      <c r="DT1" s="1" t="inlineStr">
         <is>
           <t>TXEXPRC</t>
         </is>
       </c>
-      <c r="DT1" s="1" t="inlineStr">
+      <c r="DU1" s="1" t="inlineStr">
         <is>
           <t>TXRECRC</t>
         </is>
       </c>
-      <c r="DU1" s="1" t="inlineStr">
+      <c r="DV1" s="1" t="inlineStr">
         <is>
           <t>AMTRECTAX</t>
         </is>
       </c>
-      <c r="DV1" s="1" t="inlineStr">
+      <c r="DW1" s="1" t="inlineStr">
         <is>
           <t>AMTEXPTAX</t>
         </is>
       </c>
-      <c r="DW1" s="1" t="inlineStr">
+      <c r="DX1" s="1" t="inlineStr">
         <is>
           <t>TXBSE1HC</t>
         </is>
       </c>
-      <c r="DX1" s="1" t="inlineStr">
+      <c r="DY1" s="1" t="inlineStr">
         <is>
           <t>TXBSE2HC</t>
         </is>
       </c>
-      <c r="DY1" s="1" t="inlineStr">
+      <c r="DZ1" s="1" t="inlineStr">
         <is>
           <t>TXBSE3HC</t>
         </is>
       </c>
-      <c r="DZ1" s="1" t="inlineStr">
+      <c r="EA1" s="1" t="inlineStr">
         <is>
           <t>TXBSE4HC</t>
         </is>
       </c>
-      <c r="EA1" s="1" t="inlineStr">
+      <c r="EB1" s="1" t="inlineStr">
         <is>
           <t>TXBSE5HC</t>
         </is>
       </c>
-      <c r="EB1" s="1" t="inlineStr">
+      <c r="EC1" s="1" t="inlineStr">
         <is>
           <t>TXAMT1HC</t>
         </is>
       </c>
-      <c r="EC1" s="1" t="inlineStr">
+      <c r="ED1" s="1" t="inlineStr">
         <is>
           <t>TXAMT2HC</t>
         </is>
       </c>
-      <c r="ED1" s="1" t="inlineStr">
+      <c r="EE1" s="1" t="inlineStr">
         <is>
           <t>TXAMT3HC</t>
         </is>
       </c>
-      <c r="EE1" s="1" t="inlineStr">
+      <c r="EF1" s="1" t="inlineStr">
         <is>
           <t>TXAMT4HC</t>
         </is>
       </c>
-      <c r="EF1" s="1" t="inlineStr">
+      <c r="EG1" s="1" t="inlineStr">
         <is>
           <t>TXAMT5HC</t>
         </is>
       </c>
-      <c r="EG1" s="1" t="inlineStr">
+      <c r="EH1" s="1" t="inlineStr">
         <is>
           <t>ACCTREC1</t>
         </is>
       </c>
-      <c r="EH1" s="1" t="inlineStr">
+      <c r="EI1" s="1" t="inlineStr">
         <is>
           <t>ACCTREC2</t>
         </is>
       </c>
-      <c r="EI1" s="1" t="inlineStr">
+      <c r="EJ1" s="1" t="inlineStr">
         <is>
           <t>ACCTREC3</t>
         </is>
       </c>
-      <c r="EJ1" s="1" t="inlineStr">
+      <c r="EK1" s="1" t="inlineStr">
         <is>
           <t>ACCTREC4</t>
         </is>
       </c>
-      <c r="EK1" s="1" t="inlineStr">
+      <c r="EL1" s="1" t="inlineStr">
         <is>
           <t>ACCTREC5</t>
         </is>
       </c>
-      <c r="EL1" s="1" t="inlineStr">
+      <c r="EM1" s="1" t="inlineStr">
         <is>
           <t>ACCTEXP1</t>
         </is>
       </c>
-      <c r="EM1" s="1" t="inlineStr">
+      <c r="EN1" s="1" t="inlineStr">
         <is>
           <t>ACCTEXP2</t>
         </is>
       </c>
-      <c r="EN1" s="1" t="inlineStr">
+      <c r="EO1" s="1" t="inlineStr">
         <is>
           <t>ACCTEXP3</t>
         </is>
       </c>
-      <c r="EO1" s="1" t="inlineStr">
+      <c r="EP1" s="1" t="inlineStr">
         <is>
           <t>ACCTEXP4</t>
         </is>
       </c>
-      <c r="EP1" s="1" t="inlineStr">
+      <c r="EQ1" s="1" t="inlineStr">
         <is>
           <t>ACCTEXP5</t>
         </is>
       </c>
-      <c r="EQ1" s="1" t="inlineStr">
+      <c r="ER1" s="1" t="inlineStr">
         <is>
           <t>TXEXCLTC</t>
         </is>
       </c>
-      <c r="ER1" s="1" t="inlineStr">
+      <c r="ES1" s="1" t="inlineStr">
         <is>
           <t>TXEXCLHC</t>
         </is>
       </c>
-      <c r="ES1" s="1" t="inlineStr">
+      <c r="ET1" s="1" t="inlineStr">
         <is>
           <t>TXEXCLBC</t>
         </is>
       </c>
-      <c r="ET1" s="1" t="inlineStr">
+      <c r="EU1" s="1" t="inlineStr">
         <is>
           <t>TXEXCLMC</t>
         </is>
       </c>
-      <c r="EU1" s="1" t="inlineStr">
+      <c r="EV1" s="1" t="inlineStr">
         <is>
           <t>TXINCLTC</t>
         </is>
       </c>
-      <c r="EV1" s="1" t="inlineStr">
+      <c r="EW1" s="1" t="inlineStr">
         <is>
           <t>TXINCLHC</t>
         </is>
       </c>
-      <c r="EW1" s="1" t="inlineStr">
+      <c r="EX1" s="1" t="inlineStr">
         <is>
           <t>TXINCLBC</t>
         </is>
       </c>
-      <c r="EX1" s="1" t="inlineStr">
+      <c r="EY1" s="1" t="inlineStr">
         <is>
           <t>TXINCLMC</t>
         </is>
       </c>
-      <c r="EY1" s="1" t="inlineStr">
+      <c r="EZ1" s="1" t="inlineStr">
         <is>
           <t>ARAPBATCH</t>
         </is>
       </c>
-      <c r="EZ1" s="1" t="inlineStr">
+      <c r="FA1" s="1" t="inlineStr">
         <is>
           <t>ARAPENTRY</t>
         </is>
       </c>
-      <c r="FA1" s="1" t="inlineStr">
+      <c r="FB1" s="1" t="inlineStr">
         <is>
           <t>SWCHEQUE</t>
         </is>
       </c>
-      <c r="FB1" s="1" t="inlineStr">
+      <c r="FC1" s="1" t="inlineStr">
         <is>
           <t>SWEFT</t>
         </is>
       </c>
-      <c r="FC1" s="1" t="inlineStr">
+      <c r="FD1" s="1" t="inlineStr">
         <is>
           <t>RXMTCHSEQ</t>
         </is>
       </c>
-      <c r="FD1" s="1" t="inlineStr">
+      <c r="FE1" s="1" t="inlineStr">
         <is>
           <t>RXTRNSCODE</t>
         </is>
       </c>
-      <c r="FE1" s="1" t="inlineStr">
+      <c r="FF1" s="1" t="inlineStr">
         <is>
           <t>RXCATEGORY</t>
         </is>
       </c>
-      <c r="FF1" s="1" t="inlineStr">
+      <c r="FG1" s="1" t="inlineStr">
         <is>
           <t>REVUNIQ</t>
         </is>
       </c>
-      <c r="FG1" s="1" t="inlineStr">
+      <c r="FH1" s="1" t="inlineStr">
         <is>
           <t>NEWREVUNIQ</t>
         </is>
       </c>
-      <c r="FH1" s="1" t="inlineStr">
+      <c r="FI1" s="1" t="inlineStr">
         <is>
           <t>ENTEREDBY</t>
         </is>
       </c>
-      <c r="FI1" s="1" t="inlineStr">
+      <c r="FJ1" s="1" t="inlineStr">
         <is>
           <t>WORKDESC</t>
         </is>
       </c>
-      <c r="FJ1" s="1" t="inlineStr">
+      <c r="FK1" s="1" t="inlineStr">
         <is>
           <t>BTYPE</t>
         </is>
       </c>
-      <c r="FK1" s="1" t="inlineStr">
+      <c r="FL1" s="1" t="inlineStr">
         <is>
           <t>MSCURR</t>
         </is>
       </c>
-      <c r="FL1" s="1" t="inlineStr">
+      <c r="FM1" s="1" t="inlineStr">
         <is>
           <t>BALDUE</t>
         </is>
       </c>
-      <c r="FM1" s="1" t="inlineStr">
+      <c r="FN1" s="1" t="inlineStr">
         <is>
           <t>BKCURR</t>
         </is>
       </c>
-      <c r="FN1" s="1" t="inlineStr">
+      <c r="FO1" s="1" t="inlineStr">
         <is>
           <t>SWGLQTY</t>
         </is>
       </c>
-      <c r="FO1" s="1" t="inlineStr">
+      <c r="FP1" s="1" t="inlineStr">
         <is>
           <t>GLQTYDEC</t>
         </is>
       </c>
-      <c r="FP1" s="1" t="inlineStr">
+      <c r="FQ1" s="1" t="inlineStr">
         <is>
           <t>CBBCTLRVH</t>
         </is>
       </c>
-      <c r="FQ1" s="1" t="inlineStr">
+      <c r="FR1" s="1" t="inlineStr">
         <is>
           <t>CBBCTLVW</t>
         </is>
       </c>
-      <c r="FR1" s="1" t="inlineStr">
+      <c r="FS1" s="1" t="inlineStr">
         <is>
           <t>CBBTDTRVH</t>
         </is>
       </c>
-      <c r="FS1" s="1" t="inlineStr">
+      <c r="FT1" s="1" t="inlineStr">
         <is>
           <t>CBBTDTVW</t>
         </is>
       </c>
-      <c r="FT1" s="1" t="inlineStr">
+      <c r="FU1" s="1" t="inlineStr">
         <is>
           <t>CBERRNUM</t>
         </is>
       </c>
-      <c r="FU1" s="1" t="inlineStr">
+      <c r="FV1" s="1" t="inlineStr">
         <is>
           <t>CBERRDESC</t>
         </is>
       </c>
-      <c r="FV1" s="1" t="inlineStr">
+      <c r="FW1" s="1" t="inlineStr">
         <is>
           <t>CBERRFUNC</t>
         </is>
       </c>
-      <c r="FW1" s="1" t="inlineStr">
+      <c r="FX1" s="1" t="inlineStr">
         <is>
           <t>NOVALTXGRP</t>
         </is>
@@ -1337,202 +1342,202 @@
           <t>102</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>625763</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>00001</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>AA6670348</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>05</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="n">
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
         <v>445579</v>
       </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
       <c r="Q2" t="n">
         <v>0</v>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="V2" t="n">
-        <v>1</v>
-      </c>
       <c r="W2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
         <v>1</v>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="AD2" t="n">
-        <v>1</v>
-      </c>
       <c r="AE2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="n">
         <v>1</v>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AH2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="AJ2" t="inlineStr">
+      <c r="AK2" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="AL2" t="n">
-        <v>1</v>
-      </c>
       <c r="AM2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO2" t="n">
         <v>1</v>
       </c>
-      <c r="AP2" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AQ2" t="n">
-        <v>2</v>
+      <c r="AP2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
       </c>
       <c r="AR2" t="n">
         <v>2</v>
       </c>
-      <c r="AS2" t="inlineStr"/>
+      <c r="AS2" t="n">
+        <v>2</v>
+      </c>
       <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="n">
-        <v>0</v>
-      </c>
+      <c r="AU2" t="inlineStr"/>
       <c r="AV2" t="n">
         <v>0</v>
       </c>
       <c r="AW2" t="n">
         <v>0</v>
       </c>
-      <c r="AX2" t="inlineStr"/>
-      <c r="AY2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ2" t="inlineStr"/>
-      <c r="BA2" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="BB2" t="n">
+      <c r="AX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="BC2" t="n">
         <v>2024</v>
       </c>
-      <c r="BC2" t="inlineStr"/>
-      <c r="BD2" t="inlineStr">
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr">
         <is>
           <t>AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA=</t>
         </is>
       </c>
-      <c r="BE2" t="inlineStr"/>
       <c r="BF2" t="inlineStr"/>
       <c r="BG2" t="inlineStr"/>
       <c r="BH2" t="inlineStr"/>
-      <c r="BI2" t="n">
-        <v>0</v>
-      </c>
+      <c r="BI2" t="inlineStr"/>
       <c r="BJ2" t="n">
-        <v>445579</v>
+        <v>0</v>
       </c>
       <c r="BK2" t="n">
         <v>445579</v>
@@ -1543,7 +1548,9 @@
       <c r="BM2" t="n">
         <v>445579</v>
       </c>
-      <c r="BN2" t="inlineStr"/>
+      <c r="BN2" t="n">
+        <v>445579</v>
+      </c>
       <c r="BO2" t="inlineStr"/>
       <c r="BP2" t="inlineStr"/>
       <c r="BQ2" t="inlineStr"/>
@@ -1555,9 +1562,7 @@
       <c r="BW2" t="inlineStr"/>
       <c r="BX2" t="inlineStr"/>
       <c r="BY2" t="inlineStr"/>
-      <c r="BZ2" t="n">
-        <v>1</v>
-      </c>
+      <c r="BZ2" t="inlineStr"/>
       <c r="CA2" t="n">
         <v>1</v>
       </c>
@@ -1571,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="CE2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF2" t="n">
         <v>0</v>
@@ -1615,19 +1620,19 @@
       <c r="CS2" t="n">
         <v>0</v>
       </c>
-      <c r="CT2" t="inlineStr">
+      <c r="CT2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU2" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="CU2" t="inlineStr">
+      <c r="CV2" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="CV2" t="n">
-        <v>0</v>
-      </c>
       <c r="CW2" t="n">
         <v>0</v>
       </c>
@@ -1647,41 +1652,41 @@
         <v>0</v>
       </c>
       <c r="DC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DD2" t="n">
         <v>2</v>
       </c>
-      <c r="DD2" t="n">
-        <v>1</v>
-      </c>
       <c r="DE2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DF2" t="n">
         <v>0</v>
       </c>
       <c r="DG2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DH2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="DH2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI2" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="DI2" t="n">
-        <v>1</v>
-      </c>
-      <c r="DJ2" t="inlineStr">
+      <c r="DJ2" t="n">
+        <v>1</v>
+      </c>
+      <c r="DK2" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="DK2" t="inlineStr">
+      <c r="DL2" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="DL2" t="n">
-        <v>0</v>
-      </c>
       <c r="DM2" t="n">
         <v>0</v>
       </c>
@@ -1742,7 +1747,9 @@
       <c r="EF2" t="n">
         <v>0</v>
       </c>
-      <c r="EG2" t="inlineStr"/>
+      <c r="EG2" t="n">
+        <v>0</v>
+      </c>
       <c r="EH2" t="inlineStr"/>
       <c r="EI2" t="inlineStr"/>
       <c r="EJ2" t="inlineStr"/>
@@ -1752,9 +1759,7 @@
       <c r="EN2" t="inlineStr"/>
       <c r="EO2" t="inlineStr"/>
       <c r="EP2" t="inlineStr"/>
-      <c r="EQ2" t="n">
-        <v>0</v>
-      </c>
+      <c r="EQ2" t="inlineStr"/>
       <c r="ER2" t="n">
         <v>0</v>
       </c>
@@ -1776,71 +1781,74 @@
       <c r="EX2" t="n">
         <v>0</v>
       </c>
-      <c r="EY2" t="inlineStr"/>
+      <c r="EY2" t="n">
+        <v>0</v>
+      </c>
       <c r="EZ2" t="inlineStr"/>
-      <c r="FA2" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
+      <c r="FA2" t="inlineStr"/>
       <c r="FB2" t="inlineStr">
         <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="FC2" t="inlineStr">
+        <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="FC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FD2" t="inlineStr"/>
+      <c r="FD2" t="n">
+        <v>0</v>
+      </c>
       <c r="FE2" t="inlineStr"/>
-      <c r="FF2" t="n">
-        <v>0</v>
-      </c>
+      <c r="FF2" t="inlineStr"/>
       <c r="FG2" t="n">
         <v>0</v>
       </c>
-      <c r="FH2" t="inlineStr">
+      <c r="FH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="FI2" t="inlineStr">
         <is>
           <t>TASHI</t>
         </is>
       </c>
-      <c r="FI2" t="inlineStr"/>
-      <c r="FJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FK2" t="inlineStr"/>
-      <c r="FL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FM2" t="inlineStr">
+      <c r="FJ2" t="inlineStr"/>
+      <c r="FK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="FL2" t="inlineStr"/>
+      <c r="FM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="FN2" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="FN2" t="n">
-        <v>0</v>
-      </c>
       <c r="FO2" t="n">
         <v>0</v>
       </c>
       <c r="FP2" t="n">
-        <v>241175188</v>
+        <v>0</v>
       </c>
       <c r="FQ2" t="n">
         <v>241175188</v>
       </c>
       <c r="FR2" t="n">
-        <v>241165428</v>
+        <v>241175188</v>
       </c>
       <c r="FS2" t="n">
         <v>241165428</v>
       </c>
       <c r="FT2" t="n">
-        <v>0</v>
-      </c>
-      <c r="FU2" t="inlineStr"/>
+        <v>241165428</v>
+      </c>
+      <c r="FU2" t="n">
+        <v>0</v>
+      </c>
       <c r="FV2" t="inlineStr"/>
-      <c r="FW2" t="inlineStr">
+      <c r="FW2" t="inlineStr"/>
+      <c r="FX2" t="inlineStr">
         <is>
           <t>FALSE</t>
         </is>
@@ -1852,202 +1860,202 @@
           <t>109</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>625763</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>00002</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>AC3310119</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>05</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
         <v>203480</v>
       </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="V3" t="n">
-        <v>1</v>
-      </c>
       <c r="W3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
         <v>1</v>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="Z3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AC3" t="inlineStr">
+      <c r="AD3" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="AD3" t="n">
-        <v>1</v>
-      </c>
       <c r="AE3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="n">
         <v>1</v>
       </c>
-      <c r="AH3" t="inlineStr">
+      <c r="AH3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI3" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AI3" t="inlineStr">
+      <c r="AJ3" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="AJ3" t="inlineStr">
+      <c r="AK3" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AK3" t="inlineStr">
+      <c r="AL3" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="AL3" t="n">
-        <v>1</v>
-      </c>
       <c r="AM3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO3" t="n">
         <v>1</v>
       </c>
-      <c r="AP3" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AQ3" t="n">
-        <v>2</v>
+      <c r="AP3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
       </c>
       <c r="AR3" t="n">
         <v>2</v>
       </c>
-      <c r="AS3" t="inlineStr"/>
+      <c r="AS3" t="n">
+        <v>2</v>
+      </c>
       <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AU3" t="inlineStr"/>
       <c r="AV3" t="n">
         <v>0</v>
       </c>
       <c r="AW3" t="n">
         <v>0</v>
       </c>
-      <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ3" t="inlineStr"/>
-      <c r="BA3" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="BB3" t="n">
+      <c r="AX3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA3" t="inlineStr"/>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="BC3" t="n">
         <v>2024</v>
       </c>
-      <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="inlineStr">
+      <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="inlineStr">
         <is>
           <t>AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA=</t>
         </is>
       </c>
-      <c r="BE3" t="inlineStr"/>
       <c r="BF3" t="inlineStr"/>
       <c r="BG3" t="inlineStr"/>
       <c r="BH3" t="inlineStr"/>
-      <c r="BI3" t="n">
-        <v>0</v>
-      </c>
+      <c r="BI3" t="inlineStr"/>
       <c r="BJ3" t="n">
-        <v>203480</v>
+        <v>0</v>
       </c>
       <c r="BK3" t="n">
         <v>203480</v>
@@ -2058,7 +2066,9 @@
       <c r="BM3" t="n">
         <v>203480</v>
       </c>
-      <c r="BN3" t="inlineStr"/>
+      <c r="BN3" t="n">
+        <v>203480</v>
+      </c>
       <c r="BO3" t="inlineStr"/>
       <c r="BP3" t="inlineStr"/>
       <c r="BQ3" t="inlineStr"/>
@@ -2070,9 +2080,7 @@
       <c r="BW3" t="inlineStr"/>
       <c r="BX3" t="inlineStr"/>
       <c r="BY3" t="inlineStr"/>
-      <c r="BZ3" t="n">
-        <v>1</v>
-      </c>
+      <c r="BZ3" t="inlineStr"/>
       <c r="CA3" t="n">
         <v>1</v>
       </c>
@@ -2086,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="CE3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF3" t="n">
         <v>0</v>
@@ -2130,19 +2138,19 @@
       <c r="CS3" t="n">
         <v>0</v>
       </c>
-      <c r="CT3" t="inlineStr">
+      <c r="CT3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU3" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="CU3" t="inlineStr">
+      <c r="CV3" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="CV3" t="n">
-        <v>0</v>
-      </c>
       <c r="CW3" t="n">
         <v>0</v>
       </c>
@@ -2162,41 +2170,41 @@
         <v>0</v>
       </c>
       <c r="DC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DD3" t="n">
         <v>2</v>
       </c>
-      <c r="DD3" t="n">
-        <v>1</v>
-      </c>
       <c r="DE3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DF3" t="n">
         <v>0</v>
       </c>
       <c r="DG3" t="n">
-        <v>1</v>
-      </c>
-      <c r="DH3" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="DH3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI3" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="DI3" t="n">
-        <v>1</v>
-      </c>
-      <c r="DJ3" t="inlineStr">
+      <c r="DJ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DK3" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="DK3" t="inlineStr">
+      <c r="DL3" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="DL3" t="n">
-        <v>0</v>
-      </c>
       <c r="DM3" t="n">
         <v>0</v>
       </c>
@@ -2257,7 +2265,9 @@
       <c r="EF3" t="n">
         <v>0</v>
       </c>
-      <c r="EG3" t="inlineStr"/>
+      <c r="EG3" t="n">
+        <v>0</v>
+      </c>
       <c r="EH3" t="inlineStr"/>
       <c r="EI3" t="inlineStr"/>
       <c r="EJ3" t="inlineStr"/>
@@ -2267,9 +2277,7 @@
       <c r="EN3" t="inlineStr"/>
       <c r="EO3" t="inlineStr"/>
       <c r="EP3" t="inlineStr"/>
-      <c r="EQ3" t="n">
-        <v>0</v>
-      </c>
+      <c r="EQ3" t="inlineStr"/>
       <c r="ER3" t="n">
         <v>0</v>
       </c>
@@ -2291,71 +2299,74 @@
       <c r="EX3" t="n">
         <v>0</v>
       </c>
-      <c r="EY3" t="inlineStr"/>
+      <c r="EY3" t="n">
+        <v>0</v>
+      </c>
       <c r="EZ3" t="inlineStr"/>
-      <c r="FA3" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
+      <c r="FA3" t="inlineStr"/>
       <c r="FB3" t="inlineStr">
         <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="FC3" t="inlineStr">
+        <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="FC3" t="n">
-        <v>0</v>
-      </c>
-      <c r="FD3" t="inlineStr"/>
+      <c r="FD3" t="n">
+        <v>0</v>
+      </c>
       <c r="FE3" t="inlineStr"/>
-      <c r="FF3" t="n">
-        <v>0</v>
-      </c>
+      <c r="FF3" t="inlineStr"/>
       <c r="FG3" t="n">
         <v>0</v>
       </c>
-      <c r="FH3" t="inlineStr">
+      <c r="FH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="FI3" t="inlineStr">
         <is>
           <t>TASHI</t>
         </is>
       </c>
-      <c r="FI3" t="inlineStr"/>
-      <c r="FJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="FK3" t="inlineStr"/>
-      <c r="FL3" t="n">
-        <v>0</v>
-      </c>
-      <c r="FM3" t="inlineStr">
+      <c r="FJ3" t="inlineStr"/>
+      <c r="FK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="FL3" t="inlineStr"/>
+      <c r="FM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="FN3" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="FN3" t="n">
-        <v>0</v>
-      </c>
       <c r="FO3" t="n">
         <v>0</v>
       </c>
       <c r="FP3" t="n">
-        <v>241175188</v>
+        <v>0</v>
       </c>
       <c r="FQ3" t="n">
         <v>241175188</v>
       </c>
       <c r="FR3" t="n">
-        <v>241165428</v>
+        <v>241175188</v>
       </c>
       <c r="FS3" t="n">
         <v>241165428</v>
       </c>
       <c r="FT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="FU3" t="inlineStr"/>
+        <v>241165428</v>
+      </c>
+      <c r="FU3" t="n">
+        <v>0</v>
+      </c>
       <c r="FV3" t="inlineStr"/>
-      <c r="FW3" t="inlineStr">
+      <c r="FW3" t="inlineStr"/>
+      <c r="FX3" t="inlineStr">
         <is>
           <t>FALSE</t>
         </is>
@@ -2367,202 +2378,202 @@
           <t>111</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>625763</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>00003</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>AA6670122</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>05</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="n">
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
         <v>400625</v>
       </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="V4" t="n">
-        <v>1</v>
-      </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
         <v>1</v>
       </c>
-      <c r="Z4" t="inlineStr">
+      <c r="Z4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AB4" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="AB4" t="inlineStr">
+      <c r="AC4" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AC4" t="inlineStr">
+      <c r="AD4" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="AD4" t="n">
-        <v>1</v>
-      </c>
       <c r="AE4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4" t="n">
         <v>1</v>
       </c>
-      <c r="AH4" t="inlineStr">
+      <c r="AH4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI4" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AI4" t="inlineStr">
+      <c r="AJ4" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="AJ4" t="inlineStr">
+      <c r="AK4" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AK4" t="inlineStr">
+      <c r="AL4" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="AL4" t="n">
-        <v>1</v>
-      </c>
       <c r="AM4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO4" t="n">
         <v>1</v>
       </c>
-      <c r="AP4" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AQ4" t="n">
-        <v>2</v>
+      <c r="AP4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
       </c>
       <c r="AR4" t="n">
         <v>2</v>
       </c>
-      <c r="AS4" t="inlineStr"/>
+      <c r="AS4" t="n">
+        <v>2</v>
+      </c>
       <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="n">
-        <v>0</v>
-      </c>
+      <c r="AU4" t="inlineStr"/>
       <c r="AV4" t="n">
         <v>0</v>
       </c>
       <c r="AW4" t="n">
         <v>0</v>
       </c>
-      <c r="AX4" t="inlineStr"/>
-      <c r="AY4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ4" t="inlineStr"/>
-      <c r="BA4" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="BB4" t="n">
+      <c r="AX4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="BC4" t="n">
         <v>2024</v>
       </c>
-      <c r="BC4" t="inlineStr"/>
-      <c r="BD4" t="inlineStr">
+      <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr">
         <is>
           <t>AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA=</t>
         </is>
       </c>
-      <c r="BE4" t="inlineStr"/>
       <c r="BF4" t="inlineStr"/>
       <c r="BG4" t="inlineStr"/>
       <c r="BH4" t="inlineStr"/>
-      <c r="BI4" t="n">
-        <v>0</v>
-      </c>
+      <c r="BI4" t="inlineStr"/>
       <c r="BJ4" t="n">
-        <v>400625</v>
+        <v>0</v>
       </c>
       <c r="BK4" t="n">
         <v>400625</v>
@@ -2573,7 +2584,9 @@
       <c r="BM4" t="n">
         <v>400625</v>
       </c>
-      <c r="BN4" t="inlineStr"/>
+      <c r="BN4" t="n">
+        <v>400625</v>
+      </c>
       <c r="BO4" t="inlineStr"/>
       <c r="BP4" t="inlineStr"/>
       <c r="BQ4" t="inlineStr"/>
@@ -2585,9 +2598,7 @@
       <c r="BW4" t="inlineStr"/>
       <c r="BX4" t="inlineStr"/>
       <c r="BY4" t="inlineStr"/>
-      <c r="BZ4" t="n">
-        <v>1</v>
-      </c>
+      <c r="BZ4" t="inlineStr"/>
       <c r="CA4" t="n">
         <v>1</v>
       </c>
@@ -2601,7 +2612,7 @@
         <v>1</v>
       </c>
       <c r="CE4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF4" t="n">
         <v>0</v>
@@ -2645,19 +2656,19 @@
       <c r="CS4" t="n">
         <v>0</v>
       </c>
-      <c r="CT4" t="inlineStr">
+      <c r="CT4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU4" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="CU4" t="inlineStr">
+      <c r="CV4" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="CV4" t="n">
-        <v>0</v>
-      </c>
       <c r="CW4" t="n">
         <v>0</v>
       </c>
@@ -2677,41 +2688,41 @@
         <v>0</v>
       </c>
       <c r="DC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DD4" t="n">
         <v>2</v>
       </c>
-      <c r="DD4" t="n">
-        <v>1</v>
-      </c>
       <c r="DE4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DF4" t="n">
         <v>0</v>
       </c>
       <c r="DG4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DH4" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="DH4" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI4" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="DI4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DJ4" t="inlineStr">
+      <c r="DJ4" t="n">
+        <v>1</v>
+      </c>
+      <c r="DK4" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="DK4" t="inlineStr">
+      <c r="DL4" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="DL4" t="n">
-        <v>0</v>
-      </c>
       <c r="DM4" t="n">
         <v>0</v>
       </c>
@@ -2772,7 +2783,9 @@
       <c r="EF4" t="n">
         <v>0</v>
       </c>
-      <c r="EG4" t="inlineStr"/>
+      <c r="EG4" t="n">
+        <v>0</v>
+      </c>
       <c r="EH4" t="inlineStr"/>
       <c r="EI4" t="inlineStr"/>
       <c r="EJ4" t="inlineStr"/>
@@ -2782,9 +2795,7 @@
       <c r="EN4" t="inlineStr"/>
       <c r="EO4" t="inlineStr"/>
       <c r="EP4" t="inlineStr"/>
-      <c r="EQ4" t="n">
-        <v>0</v>
-      </c>
+      <c r="EQ4" t="inlineStr"/>
       <c r="ER4" t="n">
         <v>0</v>
       </c>
@@ -2806,71 +2817,74 @@
       <c r="EX4" t="n">
         <v>0</v>
       </c>
-      <c r="EY4" t="inlineStr"/>
+      <c r="EY4" t="n">
+        <v>0</v>
+      </c>
       <c r="EZ4" t="inlineStr"/>
-      <c r="FA4" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
+      <c r="FA4" t="inlineStr"/>
       <c r="FB4" t="inlineStr">
         <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="FC4" t="inlineStr">
+        <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="FC4" t="n">
-        <v>0</v>
-      </c>
-      <c r="FD4" t="inlineStr"/>
+      <c r="FD4" t="n">
+        <v>0</v>
+      </c>
       <c r="FE4" t="inlineStr"/>
-      <c r="FF4" t="n">
-        <v>0</v>
-      </c>
+      <c r="FF4" t="inlineStr"/>
       <c r="FG4" t="n">
         <v>0</v>
       </c>
-      <c r="FH4" t="inlineStr">
+      <c r="FH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="FI4" t="inlineStr">
         <is>
           <t>TASHI</t>
         </is>
       </c>
-      <c r="FI4" t="inlineStr"/>
-      <c r="FJ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="FK4" t="inlineStr"/>
-      <c r="FL4" t="n">
-        <v>0</v>
-      </c>
-      <c r="FM4" t="inlineStr">
+      <c r="FJ4" t="inlineStr"/>
+      <c r="FK4" t="n">
+        <v>0</v>
+      </c>
+      <c r="FL4" t="inlineStr"/>
+      <c r="FM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="FN4" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="FN4" t="n">
-        <v>0</v>
-      </c>
       <c r="FO4" t="n">
         <v>0</v>
       </c>
       <c r="FP4" t="n">
-        <v>241175188</v>
+        <v>0</v>
       </c>
       <c r="FQ4" t="n">
         <v>241175188</v>
       </c>
       <c r="FR4" t="n">
-        <v>241165428</v>
+        <v>241175188</v>
       </c>
       <c r="FS4" t="n">
         <v>241165428</v>
       </c>
       <c r="FT4" t="n">
-        <v>0</v>
-      </c>
-      <c r="FU4" t="inlineStr"/>
+        <v>241165428</v>
+      </c>
+      <c r="FU4" t="n">
+        <v>0</v>
+      </c>
       <c r="FV4" t="inlineStr"/>
-      <c r="FW4" t="inlineStr">
+      <c r="FW4" t="inlineStr"/>
+      <c r="FX4" t="inlineStr">
         <is>
           <t>FALSE</t>
         </is>
@@ -2882,202 +2896,202 @@
           <t>115</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>625763</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>00004</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>AA6687758</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>05</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="n">
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
         <v>361515</v>
       </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
       <c r="Q5" t="n">
         <v>0</v>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="V5" t="n">
-        <v>1</v>
-      </c>
       <c r="W5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
         <v>1</v>
       </c>
-      <c r="Z5" t="inlineStr">
+      <c r="Z5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AA5" t="inlineStr">
+      <c r="AB5" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="AB5" t="inlineStr">
+      <c r="AC5" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AC5" t="inlineStr">
+      <c r="AD5" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="AD5" t="n">
-        <v>1</v>
-      </c>
       <c r="AE5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="n">
         <v>1</v>
       </c>
-      <c r="AH5" t="inlineStr">
+      <c r="AH5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI5" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AI5" t="inlineStr">
+      <c r="AJ5" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="AJ5" t="inlineStr">
+      <c r="AK5" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="AK5" t="inlineStr">
+      <c r="AL5" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="AL5" t="n">
-        <v>1</v>
-      </c>
       <c r="AM5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO5" t="n">
         <v>1</v>
       </c>
-      <c r="AP5" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AQ5" t="n">
-        <v>2</v>
+      <c r="AP5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
       </c>
       <c r="AR5" t="n">
         <v>2</v>
       </c>
-      <c r="AS5" t="inlineStr"/>
+      <c r="AS5" t="n">
+        <v>2</v>
+      </c>
       <c r="AT5" t="inlineStr"/>
-      <c r="AU5" t="n">
-        <v>0</v>
-      </c>
+      <c r="AU5" t="inlineStr"/>
       <c r="AV5" t="n">
         <v>0</v>
       </c>
       <c r="AW5" t="n">
         <v>0</v>
       </c>
-      <c r="AX5" t="inlineStr"/>
-      <c r="AY5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ5" t="inlineStr"/>
-      <c r="BA5" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="BB5" t="n">
+      <c r="AX5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY5" t="inlineStr"/>
+      <c r="AZ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="BC5" t="n">
         <v>2024</v>
       </c>
-      <c r="BC5" t="inlineStr"/>
-      <c r="BD5" t="inlineStr">
+      <c r="BD5" t="inlineStr"/>
+      <c r="BE5" t="inlineStr">
         <is>
           <t>AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA=</t>
         </is>
       </c>
-      <c r="BE5" t="inlineStr"/>
       <c r="BF5" t="inlineStr"/>
       <c r="BG5" t="inlineStr"/>
       <c r="BH5" t="inlineStr"/>
-      <c r="BI5" t="n">
-        <v>0</v>
-      </c>
+      <c r="BI5" t="inlineStr"/>
       <c r="BJ5" t="n">
-        <v>361515</v>
+        <v>0</v>
       </c>
       <c r="BK5" t="n">
         <v>361515</v>
@@ -3088,7 +3102,9 @@
       <c r="BM5" t="n">
         <v>361515</v>
       </c>
-      <c r="BN5" t="inlineStr"/>
+      <c r="BN5" t="n">
+        <v>361515</v>
+      </c>
       <c r="BO5" t="inlineStr"/>
       <c r="BP5" t="inlineStr"/>
       <c r="BQ5" t="inlineStr"/>
@@ -3100,9 +3116,7 @@
       <c r="BW5" t="inlineStr"/>
       <c r="BX5" t="inlineStr"/>
       <c r="BY5" t="inlineStr"/>
-      <c r="BZ5" t="n">
-        <v>1</v>
-      </c>
+      <c r="BZ5" t="inlineStr"/>
       <c r="CA5" t="n">
         <v>1</v>
       </c>
@@ -3116,7 +3130,7 @@
         <v>1</v>
       </c>
       <c r="CE5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF5" t="n">
         <v>0</v>
@@ -3160,19 +3174,19 @@
       <c r="CS5" t="n">
         <v>0</v>
       </c>
-      <c r="CT5" t="inlineStr">
+      <c r="CT5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU5" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="CU5" t="inlineStr">
+      <c r="CV5" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="CV5" t="n">
-        <v>0</v>
-      </c>
       <c r="CW5" t="n">
         <v>0</v>
       </c>
@@ -3192,41 +3206,41 @@
         <v>0</v>
       </c>
       <c r="DC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DD5" t="n">
         <v>2</v>
       </c>
-      <c r="DD5" t="n">
-        <v>1</v>
-      </c>
       <c r="DE5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DF5" t="n">
         <v>0</v>
       </c>
       <c r="DG5" t="n">
-        <v>1</v>
-      </c>
-      <c r="DH5" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="DH5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI5" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="DI5" t="n">
-        <v>1</v>
-      </c>
-      <c r="DJ5" t="inlineStr">
+      <c r="DJ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DK5" t="inlineStr">
         <is>
           <t>05/01/2024</t>
         </is>
       </c>
-      <c r="DK5" t="inlineStr">
+      <c r="DL5" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="DL5" t="n">
-        <v>0</v>
-      </c>
       <c r="DM5" t="n">
         <v>0</v>
       </c>
@@ -3287,7 +3301,9 @@
       <c r="EF5" t="n">
         <v>0</v>
       </c>
-      <c r="EG5" t="inlineStr"/>
+      <c r="EG5" t="n">
+        <v>0</v>
+      </c>
       <c r="EH5" t="inlineStr"/>
       <c r="EI5" t="inlineStr"/>
       <c r="EJ5" t="inlineStr"/>
@@ -3297,9 +3313,7 @@
       <c r="EN5" t="inlineStr"/>
       <c r="EO5" t="inlineStr"/>
       <c r="EP5" t="inlineStr"/>
-      <c r="EQ5" t="n">
-        <v>0</v>
-      </c>
+      <c r="EQ5" t="inlineStr"/>
       <c r="ER5" t="n">
         <v>0</v>
       </c>
@@ -3321,71 +3335,74 @@
       <c r="EX5" t="n">
         <v>0</v>
       </c>
-      <c r="EY5" t="inlineStr"/>
+      <c r="EY5" t="n">
+        <v>0</v>
+      </c>
       <c r="EZ5" t="inlineStr"/>
-      <c r="FA5" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
+      <c r="FA5" t="inlineStr"/>
       <c r="FB5" t="inlineStr">
         <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="FC5" t="inlineStr">
+        <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="FC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FD5" t="inlineStr"/>
+      <c r="FD5" t="n">
+        <v>0</v>
+      </c>
       <c r="FE5" t="inlineStr"/>
-      <c r="FF5" t="n">
-        <v>0</v>
-      </c>
+      <c r="FF5" t="inlineStr"/>
       <c r="FG5" t="n">
         <v>0</v>
       </c>
-      <c r="FH5" t="inlineStr">
+      <c r="FH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="FI5" t="inlineStr">
         <is>
           <t>TASHI</t>
         </is>
       </c>
-      <c r="FI5" t="inlineStr"/>
-      <c r="FJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FK5" t="inlineStr"/>
-      <c r="FL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FM5" t="inlineStr">
+      <c r="FJ5" t="inlineStr"/>
+      <c r="FK5" t="n">
+        <v>0</v>
+      </c>
+      <c r="FL5" t="inlineStr"/>
+      <c r="FM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="FN5" t="inlineStr">
         <is>
           <t>JAD</t>
         </is>
       </c>
-      <c r="FN5" t="n">
-        <v>0</v>
-      </c>
       <c r="FO5" t="n">
         <v>0</v>
       </c>
       <c r="FP5" t="n">
-        <v>241175188</v>
+        <v>0</v>
       </c>
       <c r="FQ5" t="n">
         <v>241175188</v>
       </c>
       <c r="FR5" t="n">
-        <v>241165428</v>
+        <v>241175188</v>
       </c>
       <c r="FS5" t="n">
         <v>241165428</v>
       </c>
       <c r="FT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="FU5" t="inlineStr"/>
+        <v>241165428</v>
+      </c>
+      <c r="FU5" t="n">
+        <v>0</v>
+      </c>
       <c r="FV5" t="inlineStr"/>
-      <c r="FW5" t="inlineStr">
+      <c r="FW5" t="inlineStr"/>
+      <c r="FX5" t="inlineStr">
         <is>
           <t>FALSE</t>
         </is>
@@ -4265,7 +4282,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -4774,7 +4791,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -5283,7 +5300,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -5792,7 +5809,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6301,7 +6318,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6810,7 +6827,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -7319,7 +7336,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -7828,7 +7845,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -8337,7 +8354,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -8846,7 +8863,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -9355,7 +9372,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -9864,7 +9881,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -10373,7 +10390,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -10882,7 +10899,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -11391,7 +11408,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -11900,7 +11917,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -12409,7 +12426,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -12918,7 +12935,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -13427,7 +13444,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -13936,7 +13953,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -14445,7 +14462,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -14954,7 +14971,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -15463,7 +15480,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -15972,7 +15989,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -16481,7 +16498,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -16990,7 +17007,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -17499,7 +17516,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -18008,7 +18025,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -18517,7 +18534,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -19026,7 +19043,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -19535,7 +19552,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -20044,7 +20061,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -20553,7 +20570,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -21062,7 +21079,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -21571,7 +21588,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -22080,7 +22097,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -22589,7 +22606,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -23098,7 +23115,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -23607,7 +23624,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -24116,7 +24133,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -24625,7 +24642,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -25134,7 +25151,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -25643,7 +25660,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -26152,7 +26169,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -26661,7 +26678,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -27170,7 +27187,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -27679,7 +27696,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -28188,7 +28205,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -28697,7 +28714,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -29206,7 +29223,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -29715,7 +29732,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -30224,7 +30241,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -30733,7 +30750,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -31242,7 +31259,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -31751,7 +31768,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -32260,7 +32277,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -32769,7 +32786,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -33278,7 +33295,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -33787,7 +33804,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -34296,7 +34313,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -34805,7 +34822,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -35314,7 +35331,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -35823,7 +35840,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -36332,7 +36349,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -36841,7 +36858,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -37350,7 +37367,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -37859,7 +37876,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -38368,7 +38385,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -38877,7 +38894,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -39386,7 +39403,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -39895,7 +39912,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -40404,7 +40421,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -40913,7 +40930,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -41422,7 +41439,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -41931,7 +41948,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -42440,7 +42457,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -42949,7 +42966,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -43458,7 +43475,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -43967,7 +43984,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -44476,7 +44493,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -44985,7 +45002,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -45494,7 +45511,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -46003,7 +46020,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -46512,7 +46529,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -47021,7 +47038,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -47530,7 +47547,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -48039,7 +48056,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -48548,7 +48565,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -49057,7 +49074,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -49566,7 +49583,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -50075,7 +50092,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -50584,7 +50601,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -51093,7 +51110,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -51602,7 +51619,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -52111,7 +52128,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -52620,7 +52637,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>605936</v>
+        <v>625763</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Load Store and Account Detail CSV files data into DataFrames  * Rename Store and Account Detail CSV files to follow non-plural naming conventions  * Define CSV Dictionary and assign table and file names  * Load data from CSV files into a separate DataFrames list
</commit_message>
<xml_diff>
--- a/CASH REPORT.xlsx
+++ b/CASH REPORT.xlsx
@@ -1343,7 +1343,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1861,7 +1861,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2379,7 +2379,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2897,7 +2897,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -4282,7 +4282,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -4791,7 +4791,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -5300,7 +5300,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -5809,7 +5809,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6318,7 +6318,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6827,7 +6827,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -7336,7 +7336,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -7845,7 +7845,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -8354,7 +8354,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -8863,7 +8863,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -9372,7 +9372,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -9881,7 +9881,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -10390,7 +10390,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -10899,7 +10899,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -11408,7 +11408,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -11917,7 +11917,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -12426,7 +12426,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -12935,7 +12935,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -13444,7 +13444,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -13953,7 +13953,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -14462,7 +14462,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -14971,7 +14971,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -15480,7 +15480,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -15989,7 +15989,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -16498,7 +16498,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -17007,7 +17007,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -17516,7 +17516,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -18025,7 +18025,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -18534,7 +18534,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -19043,7 +19043,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -19552,7 +19552,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -20061,7 +20061,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -20570,7 +20570,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -21079,7 +21079,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -21588,7 +21588,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -22097,7 +22097,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -22606,7 +22606,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -23115,7 +23115,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -23624,7 +23624,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -24133,7 +24133,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -24642,7 +24642,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -25151,7 +25151,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -25660,7 +25660,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -26169,7 +26169,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -26678,7 +26678,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -27187,7 +27187,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -27696,7 +27696,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -28205,7 +28205,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -28714,7 +28714,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -29223,7 +29223,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -29732,7 +29732,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -30241,7 +30241,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -30750,7 +30750,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -31259,7 +31259,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -31768,7 +31768,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -32277,7 +32277,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -32786,7 +32786,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -33295,7 +33295,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -33804,7 +33804,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -34313,7 +34313,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -34822,7 +34822,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -35331,7 +35331,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -35840,7 +35840,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -36349,7 +36349,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -36858,7 +36858,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -37367,7 +37367,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -37876,7 +37876,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -38385,7 +38385,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -38894,7 +38894,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -39403,7 +39403,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -39912,7 +39912,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -40421,7 +40421,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -40930,7 +40930,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -41439,7 +41439,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -41948,7 +41948,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -42457,7 +42457,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -42966,7 +42966,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -43475,7 +43475,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -43984,7 +43984,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -44493,7 +44493,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -45002,7 +45002,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -45511,7 +45511,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -46020,7 +46020,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -46529,7 +46529,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -47038,7 +47038,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -47547,7 +47547,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -48056,7 +48056,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -48565,7 +48565,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -49074,7 +49074,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -49583,7 +49583,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -50092,7 +50092,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -50601,7 +50601,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -51110,7 +51110,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -51619,7 +51619,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -52128,7 +52128,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -52637,7 +52637,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>625763</v>
+        <v>12389</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Assign TEXTDESC values on Batch Header sheet based on Store Detail  * Re-arrange Columns on Account Detail and Store Detail CSV so that match column is the first column  * Leverage merge method to calculate TEXTDESC values based on StoreKey and reformatted Date
</commit_message>
<xml_diff>
--- a/CASH REPORT.xlsx
+++ b/CASH REPORT.xlsx
@@ -1337,13 +1337,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="A2" t="n">
+        <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1375,7 +1373,11 @@
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>PORT BANK 01.05.2024</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
@@ -1855,13 +1857,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="A3" t="n">
+        <v>109</v>
       </c>
       <c r="B3" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1893,7 +1893,11 @@
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>BARR BANK 01.05.2024</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
@@ -2373,13 +2377,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="A4" t="n">
+        <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2411,7 +2413,11 @@
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>MAYP BANK 01.05.2024</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
@@ -2891,13 +2897,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="A5" t="n">
+        <v>115</v>
       </c>
       <c r="B5" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -2929,7 +2933,11 @@
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>UHWI BANK 01.05.2024</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
@@ -4282,7 +4290,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -4791,7 +4799,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -5300,7 +5308,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -5809,7 +5817,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6318,7 +6326,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6827,7 +6835,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -7336,7 +7344,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -7845,7 +7853,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -8354,7 +8362,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -8863,7 +8871,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -9372,7 +9380,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -9881,7 +9889,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -10390,7 +10398,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -10899,7 +10907,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -11408,7 +11416,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -11917,7 +11925,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -12426,7 +12434,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -12935,7 +12943,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -13444,7 +13452,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -13953,7 +13961,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -14462,7 +14470,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -14971,7 +14979,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -15480,7 +15488,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -15989,7 +15997,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -16498,7 +16506,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -17007,7 +17015,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -17516,7 +17524,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -18025,7 +18033,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -18534,7 +18542,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -19043,7 +19051,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -19552,7 +19560,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -20061,7 +20069,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -20570,7 +20578,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -21079,7 +21087,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -21588,7 +21596,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -22097,7 +22105,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -22606,7 +22614,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -23115,7 +23123,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -23624,7 +23632,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -24133,7 +24141,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -24642,7 +24650,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -25151,7 +25159,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -25660,7 +25668,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -26169,7 +26177,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -26678,7 +26686,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -27187,7 +27195,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -27696,7 +27704,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -28205,7 +28213,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -28714,7 +28722,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -29223,7 +29231,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -29732,7 +29740,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -30241,7 +30249,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -30750,7 +30758,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -31259,7 +31267,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -31768,7 +31776,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -32277,7 +32285,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -32786,7 +32794,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -33295,7 +33303,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -33804,7 +33812,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -34313,7 +34321,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -34822,7 +34830,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -35331,7 +35339,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -35840,7 +35848,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -36349,7 +36357,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -36858,7 +36866,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -37367,7 +37375,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -37876,7 +37884,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -38385,7 +38393,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -38894,7 +38902,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -39403,7 +39411,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -39912,7 +39920,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -40421,7 +40429,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -40930,7 +40938,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -41439,7 +41447,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -41948,7 +41956,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -42457,7 +42465,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -42966,7 +42974,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -43475,7 +43483,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -43984,7 +43992,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -44493,7 +44501,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -45002,7 +45010,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -45511,7 +45519,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -46020,7 +46028,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -46529,7 +46537,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -47038,7 +47046,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -47547,7 +47555,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -48056,7 +48064,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -48565,7 +48573,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -49074,7 +49082,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -49583,7 +49591,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -50092,7 +50100,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -50601,7 +50609,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -51110,7 +51118,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -51619,7 +51627,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -52128,7 +52136,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -52637,7 +52645,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>12389</v>
+        <v>555185</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Assign Account ID, Account Description and Text Description fields  * Set ACCTDESC to CASH SHORTAGE or OVERAGE based on negative/positve value  * Assign column values on Batch Detail sheet based on Store and Account Detail DataFrames
</commit_message>
<xml_diff>
--- a/CASH REPORT.xlsx
+++ b/CASH REPORT.xlsx
@@ -1341,7 +1341,7 @@
         <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1861,7 +1861,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2381,7 +2381,7 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2901,7 +2901,7 @@
         <v>115</v>
       </c>
       <c r="B5" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -4279,10 +4279,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="A2" t="n">
+        <v>101</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4290,7 +4288,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -4303,8 +4301,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>TCHR BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
           <t>11</t>
@@ -4788,10 +4794,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="A3" t="n">
+        <v>101</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -4799,7 +4803,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -4812,8 +4816,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>TCHR 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>11</t>
@@ -5297,10 +5309,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="A4" t="n">
+        <v>101</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -5308,7 +5318,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -5321,8 +5331,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>TCHR CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
           <t>11</t>
@@ -5806,10 +5824,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="A5" t="n">
+        <v>101</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -5817,7 +5833,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -5830,8 +5846,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>TCHR LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>11</t>
@@ -6315,10 +6339,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="A6" t="n">
+        <v>101</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -6326,7 +6348,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6339,8 +6361,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>TCHR CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr">
         <is>
           <t>11</t>
@@ -6824,10 +6854,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="A7" t="n">
+        <v>101</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -6835,7 +6863,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -6848,8 +6876,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>TCHR CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
           <t>11</t>
@@ -7333,10 +7369,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="A8" t="n">
+        <v>101</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -7344,7 +7378,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -7357,8 +7391,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>TCHR BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1740-CASH</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
           <t>11</t>
@@ -7398,7 +7440,7 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH SHORTAGE</t>
         </is>
       </c>
       <c r="Y8" t="n">
@@ -7842,10 +7884,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="A9" t="n">
+        <v>101</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -7853,7 +7893,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -7866,8 +7906,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>TCHR BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
           <t>11</t>
@@ -8351,10 +8399,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="A10" t="n">
+        <v>102</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -8362,7 +8408,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -8375,8 +8421,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>PORT BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr">
         <is>
           <t>11</t>
@@ -8860,10 +8914,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="A11" t="n">
+        <v>102</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -8871,7 +8923,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -8884,8 +8936,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>PORT 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr">
         <is>
           <t>11</t>
@@ -9369,10 +9429,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="A12" t="n">
+        <v>102</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -9380,7 +9438,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -9393,8 +9451,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>PORT CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr">
         <is>
           <t>11</t>
@@ -9878,10 +9944,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="A13" t="n">
+        <v>102</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -9889,7 +9953,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -9902,8 +9966,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>PORT LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr">
         <is>
           <t>11</t>
@@ -10387,10 +10459,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="A14" t="n">
+        <v>102</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -10398,7 +10468,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -10411,8 +10481,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>PORT CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr">
         <is>
           <t>11</t>
@@ -10896,10 +10974,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="A15" t="n">
+        <v>102</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -10907,7 +10983,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -10920,8 +10996,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>PORT CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr">
         <is>
           <t>11</t>
@@ -11405,10 +11489,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="A16" t="n">
+        <v>102</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -11416,7 +11498,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -11429,8 +11511,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>PORT BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>1740-CASH</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr">
         <is>
           <t>11</t>
@@ -11470,7 +11560,7 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH SHORTAGE</t>
         </is>
       </c>
       <c r="Y16" t="n">
@@ -11914,10 +12004,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="A17" t="n">
+        <v>102</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -11925,7 +12013,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -11938,8 +12026,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>PORT BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr">
         <is>
           <t>11</t>
@@ -12423,10 +12519,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A18" t="n">
+        <v>103</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -12434,7 +12528,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -12447,8 +12541,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>DVHS BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr">
         <is>
           <t>11</t>
@@ -12932,10 +13034,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A19" t="n">
+        <v>103</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -12943,7 +13043,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -12956,8 +13056,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>DVHS 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr">
         <is>
           <t>11</t>
@@ -13441,10 +13549,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A20" t="n">
+        <v>103</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -13452,7 +13558,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -13465,8 +13571,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>DVHS CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I20" t="inlineStr">
         <is>
           <t>11</t>
@@ -13950,10 +14064,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A21" t="n">
+        <v>103</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -13961,7 +14073,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -13974,8 +14086,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>DVHS LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr">
         <is>
           <t>11</t>
@@ -14459,10 +14579,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A22" t="n">
+        <v>103</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -14470,7 +14588,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -14483,8 +14601,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>DVHS CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr">
         <is>
           <t>11</t>
@@ -14968,10 +15094,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A23" t="n">
+        <v>103</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -14979,7 +15103,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -14992,8 +15116,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>DVHS CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr">
         <is>
           <t>11</t>
@@ -15477,10 +15609,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A24" t="n">
+        <v>103</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -15488,7 +15618,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -15501,8 +15631,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>DVHS BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>1740-CASH</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr">
         <is>
           <t>11</t>
@@ -15542,7 +15680,7 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH SHORTAGE</t>
         </is>
       </c>
       <c r="Y24" t="n">
@@ -15986,10 +16124,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A25" t="n">
+        <v>103</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -15997,7 +16133,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -16010,8 +16146,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>DVHS BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I25" t="inlineStr">
         <is>
           <t>11</t>
@@ -16495,10 +16639,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
+      <c r="A26" t="n">
+        <v>104</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -16506,7 +16648,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -16519,8 +16661,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>DBHT BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I26" t="inlineStr">
         <is>
           <t>11</t>
@@ -17004,10 +17154,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
+      <c r="A27" t="n">
+        <v>104</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -17015,7 +17163,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -17028,8 +17176,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>DBHT 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr">
         <is>
           <t>11</t>
@@ -17513,10 +17669,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
+      <c r="A28" t="n">
+        <v>104</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -17524,7 +17678,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -17537,8 +17691,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>DBHT CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I28" t="inlineStr">
         <is>
           <t>11</t>
@@ -18022,10 +18184,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
+      <c r="A29" t="n">
+        <v>104</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -18033,7 +18193,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -18046,8 +18206,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>DBHT LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr">
         <is>
           <t>11</t>
@@ -18531,10 +18699,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
+      <c r="A30" t="n">
+        <v>104</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -18542,7 +18708,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -18555,8 +18721,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>DBHT CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I30" t="inlineStr">
         <is>
           <t>11</t>
@@ -19040,10 +19214,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
+      <c r="A31" t="n">
+        <v>104</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -19051,7 +19223,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -19064,8 +19236,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>DBHT CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I31" t="inlineStr">
         <is>
           <t>11</t>
@@ -19549,10 +19729,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
+      <c r="A32" t="n">
+        <v>104</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -19560,7 +19738,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -19573,8 +19751,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>DBHT BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>1740-CASH</t>
+        </is>
+      </c>
       <c r="I32" t="inlineStr">
         <is>
           <t>11</t>
@@ -19614,7 +19800,7 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH SHORTAGE</t>
         </is>
       </c>
       <c r="Y32" t="n">
@@ -20058,10 +20244,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
+      <c r="A33" t="n">
+        <v>104</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -20069,7 +20253,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -20082,8 +20266,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>DBHT BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I33" t="inlineStr">
         <is>
           <t>11</t>
@@ -20567,10 +20759,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="A34" t="n">
+        <v>105</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -20578,7 +20768,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -20591,8 +20781,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>PARK BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I34" t="inlineStr">
         <is>
           <t>11</t>
@@ -21076,10 +21274,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="A35" t="n">
+        <v>105</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -21087,7 +21283,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -21100,8 +21296,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>PARK 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I35" t="inlineStr">
         <is>
           <t>11</t>
@@ -21585,10 +21789,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="A36" t="n">
+        <v>105</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -21596,7 +21798,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -21609,8 +21811,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>PARK CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I36" t="inlineStr">
         <is>
           <t>11</t>
@@ -22094,10 +22304,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="A37" t="n">
+        <v>105</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -22105,7 +22313,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -22118,8 +22326,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>PARK LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I37" t="inlineStr">
         <is>
           <t>11</t>
@@ -22603,10 +22819,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="A38" t="n">
+        <v>105</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -22614,7 +22828,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -22627,8 +22841,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>PARK CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I38" t="inlineStr">
         <is>
           <t>11</t>
@@ -23112,10 +23334,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="A39" t="n">
+        <v>105</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -23123,7 +23343,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -23136,8 +23356,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>PARK CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I39" t="inlineStr">
         <is>
           <t>11</t>
@@ -23621,10 +23849,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="A40" t="n">
+        <v>105</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -23632,7 +23858,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -23645,8 +23871,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>PARK BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>1740-CASH</t>
+        </is>
+      </c>
       <c r="I40" t="inlineStr">
         <is>
           <t>11</t>
@@ -23686,7 +23920,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH SHORTAGE</t>
         </is>
       </c>
       <c r="Y40" t="n">
@@ -24130,10 +24364,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>105</t>
-        </is>
+      <c r="A41" t="n">
+        <v>105</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -24141,7 +24373,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -24154,8 +24386,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>PARK BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I41" t="inlineStr">
         <is>
           <t>11</t>
@@ -24639,10 +24879,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
+      <c r="A42" t="n">
+        <v>106</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -24650,7 +24888,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -24663,8 +24901,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>NORT BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I42" t="inlineStr">
         <is>
           <t>11</t>
@@ -25148,10 +25394,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
+      <c r="A43" t="n">
+        <v>106</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -25159,7 +25403,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -25172,8 +25416,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>NORT 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr">
         <is>
           <t>11</t>
@@ -25657,10 +25909,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
+      <c r="A44" t="n">
+        <v>106</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -25668,7 +25918,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -25681,8 +25931,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>NORT CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I44" t="inlineStr">
         <is>
           <t>11</t>
@@ -26166,10 +26424,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
+      <c r="A45" t="n">
+        <v>106</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -26177,7 +26433,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -26190,8 +26446,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>NORT LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I45" t="inlineStr">
         <is>
           <t>11</t>
@@ -26675,10 +26939,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
+      <c r="A46" t="n">
+        <v>106</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -26686,7 +26948,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -26699,8 +26961,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>NORT CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I46" t="inlineStr">
         <is>
           <t>11</t>
@@ -27184,10 +27454,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
+      <c r="A47" t="n">
+        <v>106</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -27195,7 +27463,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -27208,8 +27476,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>NORT CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I47" t="inlineStr">
         <is>
           <t>11</t>
@@ -27693,10 +27969,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
+      <c r="A48" t="n">
+        <v>106</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -27704,7 +27978,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -27717,8 +27991,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>NORT BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>1740-CASH</t>
+        </is>
+      </c>
       <c r="I48" t="inlineStr">
         <is>
           <t>11</t>
@@ -27758,7 +28040,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH SHORTAGE</t>
         </is>
       </c>
       <c r="Y48" t="n">
@@ -28202,10 +28484,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
+      <c r="A49" t="n">
+        <v>106</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -28213,7 +28493,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -28226,8 +28506,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>NORT BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I49" t="inlineStr">
         <is>
           <t>11</t>
@@ -28711,10 +28999,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
+      <c r="A50" t="n">
+        <v>108</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -28722,7 +29008,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -28735,8 +29021,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>LIGN BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I50" t="inlineStr">
         <is>
           <t>11</t>
@@ -29220,10 +29514,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
+      <c r="A51" t="n">
+        <v>108</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -29231,7 +29523,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -29244,8 +29536,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>LIGN 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I51" t="inlineStr">
         <is>
           <t>11</t>
@@ -29729,10 +30029,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
+      <c r="A52" t="n">
+        <v>108</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -29740,7 +30038,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -29753,8 +30051,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>LIGN CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I52" t="inlineStr">
         <is>
           <t>11</t>
@@ -30238,10 +30544,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
+      <c r="A53" t="n">
+        <v>108</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -30249,7 +30553,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -30262,8 +30566,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>LIGN LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I53" t="inlineStr">
         <is>
           <t>11</t>
@@ -30747,10 +31059,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
+      <c r="A54" t="n">
+        <v>108</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -30758,7 +31068,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -30771,8 +31081,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>LIGN CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I54" t="inlineStr">
         <is>
           <t>11</t>
@@ -31256,10 +31574,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
+      <c r="A55" t="n">
+        <v>108</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -31267,7 +31583,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -31280,8 +31596,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>LIGN CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I55" t="inlineStr">
         <is>
           <t>11</t>
@@ -31765,10 +32089,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
+      <c r="A56" t="n">
+        <v>108</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -31776,7 +32098,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -31789,8 +32111,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>LIGN BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>4200</t>
+        </is>
+      </c>
       <c r="I56" t="inlineStr">
         <is>
           <t>11</t>
@@ -31830,7 +32160,7 @@
       </c>
       <c r="X56" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH OVERAGE</t>
         </is>
       </c>
       <c r="Y56" t="n">
@@ -32274,10 +32604,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
+      <c r="A57" t="n">
+        <v>108</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -32285,7 +32613,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -32298,8 +32626,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>LIGN BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I57" t="inlineStr">
         <is>
           <t>11</t>
@@ -32783,10 +33119,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="A58" t="n">
+        <v>109</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -32794,7 +33128,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -32807,8 +33141,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>BARR BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I58" t="inlineStr">
         <is>
           <t>11</t>
@@ -33292,10 +33634,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="A59" t="n">
+        <v>109</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -33303,7 +33643,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -33316,8 +33656,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>BARR 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I59" t="inlineStr">
         <is>
           <t>11</t>
@@ -33801,10 +34149,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="A60" t="n">
+        <v>109</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -33812,7 +34158,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -33825,8 +34171,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>BARR CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I60" t="inlineStr">
         <is>
           <t>11</t>
@@ -34310,10 +34664,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="A61" t="n">
+        <v>109</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -34321,7 +34673,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -34334,8 +34686,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>BARR LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I61" t="inlineStr">
         <is>
           <t>11</t>
@@ -34819,10 +35179,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="A62" t="n">
+        <v>109</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -34830,7 +35188,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -34843,8 +35201,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr"/>
-      <c r="H62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>BARR CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I62" t="inlineStr">
         <is>
           <t>11</t>
@@ -35328,10 +35694,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="A63" t="n">
+        <v>109</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -35339,7 +35703,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -35352,8 +35716,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr"/>
-      <c r="H63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>BARR CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I63" t="inlineStr">
         <is>
           <t>11</t>
@@ -35837,10 +36209,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="A64" t="n">
+        <v>109</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -35848,7 +36218,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -35861,8 +36231,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>BARR BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>4200</t>
+        </is>
+      </c>
       <c r="I64" t="inlineStr">
         <is>
           <t>11</t>
@@ -35902,7 +36280,7 @@
       </c>
       <c r="X64" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH OVERAGE</t>
         </is>
       </c>
       <c r="Y64" t="n">
@@ -36346,10 +36724,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="A65" t="n">
+        <v>109</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -36357,7 +36733,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -36370,8 +36746,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>BARR BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I65" t="inlineStr">
         <is>
           <t>11</t>
@@ -36855,10 +37239,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="A66" t="n">
+        <v>110</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -36866,7 +37248,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -36879,8 +37261,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr"/>
-      <c r="H66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>OCHO BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I66" t="inlineStr">
         <is>
           <t>11</t>
@@ -37364,10 +37754,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="A67" t="n">
+        <v>110</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -37375,7 +37763,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -37388,8 +37776,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>OCHO 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I67" t="inlineStr">
         <is>
           <t>11</t>
@@ -37873,10 +38269,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="A68" t="n">
+        <v>110</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -37884,7 +38278,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -37897,8 +38291,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G68" t="inlineStr"/>
-      <c r="H68" t="inlineStr"/>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>OCHO CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I68" t="inlineStr">
         <is>
           <t>11</t>
@@ -38382,10 +38784,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="A69" t="n">
+        <v>110</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -38393,7 +38793,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -38406,8 +38806,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G69" t="inlineStr"/>
-      <c r="H69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>OCHO LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I69" t="inlineStr">
         <is>
           <t>11</t>
@@ -38891,10 +39299,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="A70" t="n">
+        <v>110</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -38902,7 +39308,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -38915,8 +39321,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>OCHO CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I70" t="inlineStr">
         <is>
           <t>11</t>
@@ -39400,10 +39814,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="A71" t="n">
+        <v>110</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -39411,7 +39823,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -39424,8 +39836,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr"/>
-      <c r="H71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>OCHO CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I71" t="inlineStr">
         <is>
           <t>11</t>
@@ -39909,10 +40329,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="A72" t="n">
+        <v>110</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -39920,7 +40338,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -39933,8 +40351,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>OCHO BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>1740-CASH</t>
+        </is>
+      </c>
       <c r="I72" t="inlineStr">
         <is>
           <t>11</t>
@@ -39974,7 +40400,7 @@
       </c>
       <c r="X72" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH SHORTAGE</t>
         </is>
       </c>
       <c r="Y72" t="n">
@@ -40418,10 +40844,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="A73" t="n">
+        <v>110</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -40429,7 +40853,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -40442,8 +40866,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr"/>
-      <c r="H73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>OCHO BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I73" t="inlineStr">
         <is>
           <t>11</t>
@@ -40927,10 +41359,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="A74" t="n">
+        <v>111</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -40938,7 +41368,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -40951,8 +41381,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr"/>
-      <c r="H74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>MAYP BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I74" t="inlineStr">
         <is>
           <t>11</t>
@@ -41436,10 +41874,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="A75" t="n">
+        <v>111</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -41447,7 +41883,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -41460,8 +41896,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr"/>
-      <c r="H75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>MAYP 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I75" t="inlineStr">
         <is>
           <t>11</t>
@@ -41945,10 +42389,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="A76" t="n">
+        <v>111</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -41956,7 +42398,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -41969,8 +42411,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G76" t="inlineStr"/>
-      <c r="H76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>MAYP CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I76" t="inlineStr">
         <is>
           <t>11</t>
@@ -42454,10 +42904,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="A77" t="n">
+        <v>111</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -42465,7 +42913,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -42478,8 +42926,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G77" t="inlineStr"/>
-      <c r="H77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>MAYP LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I77" t="inlineStr">
         <is>
           <t>11</t>
@@ -42963,10 +43419,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="A78" t="n">
+        <v>111</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -42974,7 +43428,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -42987,8 +43441,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G78" t="inlineStr"/>
-      <c r="H78" t="inlineStr"/>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>MAYP CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I78" t="inlineStr">
         <is>
           <t>11</t>
@@ -43472,10 +43934,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="A79" t="n">
+        <v>111</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -43483,7 +43943,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -43496,8 +43956,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G79" t="inlineStr"/>
-      <c r="H79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>MAYP CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I79" t="inlineStr">
         <is>
           <t>11</t>
@@ -43981,10 +44449,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="A80" t="n">
+        <v>111</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -43992,7 +44458,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -44005,8 +44471,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G80" t="inlineStr"/>
-      <c r="H80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>MAYP BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>4200</t>
+        </is>
+      </c>
       <c r="I80" t="inlineStr">
         <is>
           <t>11</t>
@@ -44046,7 +44520,7 @@
       </c>
       <c r="X80" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH OVERAGE</t>
         </is>
       </c>
       <c r="Y80" t="n">
@@ -44490,10 +44964,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="A81" t="n">
+        <v>111</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -44501,7 +44973,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -44514,8 +44986,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G81" t="inlineStr"/>
-      <c r="H81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>MAYP BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I81" t="inlineStr">
         <is>
           <t>11</t>
@@ -44999,10 +45479,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="A82" t="n">
+        <v>112</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -45010,7 +45488,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -45023,8 +45501,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G82" t="inlineStr"/>
-      <c r="H82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>ANNO BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I82" t="inlineStr">
         <is>
           <t>11</t>
@@ -45508,10 +45994,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="A83" t="n">
+        <v>112</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -45519,7 +46003,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -45532,8 +46016,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>ANNO 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I83" t="inlineStr">
         <is>
           <t>11</t>
@@ -46017,10 +46509,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="A84" t="n">
+        <v>112</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -46028,7 +46518,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -46041,8 +46531,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G84" t="inlineStr"/>
-      <c r="H84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>ANNO CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I84" t="inlineStr">
         <is>
           <t>11</t>
@@ -46526,10 +47024,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="A85" t="n">
+        <v>112</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -46537,7 +47033,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -46550,8 +47046,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G85" t="inlineStr"/>
-      <c r="H85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>ANNO LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I85" t="inlineStr">
         <is>
           <t>11</t>
@@ -47035,10 +47539,8 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="A86" t="n">
+        <v>112</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -47046,7 +47548,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -47059,8 +47561,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G86" t="inlineStr"/>
-      <c r="H86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>ANNO CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I86" t="inlineStr">
         <is>
           <t>11</t>
@@ -47544,10 +48054,8 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="A87" t="n">
+        <v>112</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -47555,7 +48063,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -47568,8 +48076,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G87" t="inlineStr"/>
-      <c r="H87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>ANNO CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I87" t="inlineStr">
         <is>
           <t>11</t>
@@ -48053,10 +48569,8 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="A88" t="n">
+        <v>112</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -48064,7 +48578,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -48077,8 +48591,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G88" t="inlineStr"/>
-      <c r="H88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>ANNO BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>1740-CASH</t>
+        </is>
+      </c>
       <c r="I88" t="inlineStr">
         <is>
           <t>11</t>
@@ -48118,7 +48640,7 @@
       </c>
       <c r="X88" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH SHORTAGE</t>
         </is>
       </c>
       <c r="Y88" t="n">
@@ -48562,10 +49084,8 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="A89" t="n">
+        <v>112</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -48573,7 +49093,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -48586,8 +49106,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G89" t="inlineStr"/>
-      <c r="H89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>ANNO BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I89" t="inlineStr">
         <is>
           <t>11</t>
@@ -49071,10 +49599,8 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="A90" t="n">
+        <v>115</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -49082,7 +49608,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -49095,8 +49621,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G90" t="inlineStr"/>
-      <c r="H90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>UHWI BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>1750</t>
+        </is>
+      </c>
       <c r="I90" t="inlineStr">
         <is>
           <t>11</t>
@@ -49580,10 +50114,8 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="A91" t="n">
+        <v>115</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -49591,7 +50123,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -49604,8 +50136,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G91" t="inlineStr"/>
-      <c r="H91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>UHWI 7KRAVE 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>1740-DLVR</t>
+        </is>
+      </c>
       <c r="I91" t="inlineStr">
         <is>
           <t>11</t>
@@ -50089,10 +50629,8 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="A92" t="n">
+        <v>115</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -50100,7 +50638,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -50113,8 +50651,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G92" t="inlineStr"/>
-      <c r="H92" t="inlineStr"/>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>UHWI CORPORATE CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>1740-CORP</t>
+        </is>
+      </c>
       <c r="I92" t="inlineStr">
         <is>
           <t>11</t>
@@ -50598,10 +51144,8 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="A93" t="n">
+        <v>115</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -50609,7 +51153,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -50622,8 +51166,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G93" t="inlineStr"/>
-      <c r="H93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>UHWI LUNCH VOUCHER 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>1740-LUNCHV</t>
+        </is>
+      </c>
       <c r="I93" t="inlineStr">
         <is>
           <t>11</t>
@@ -51107,10 +51659,8 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="A94" t="n">
+        <v>115</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -51118,7 +51668,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -51131,8 +51681,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G94" t="inlineStr"/>
-      <c r="H94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>UHWI CR/DB CARD 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>1740-CREDIT</t>
+        </is>
+      </c>
       <c r="I94" t="inlineStr">
         <is>
           <t>11</t>
@@ -51616,10 +52174,8 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="A95" t="n">
+        <v>115</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -51627,7 +52183,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -51640,8 +52196,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G95" t="inlineStr"/>
-      <c r="H95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>UHWI CREDIT 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>1740-IOU</t>
+        </is>
+      </c>
       <c r="I95" t="inlineStr">
         <is>
           <t>11</t>
@@ -52125,10 +52689,8 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="A96" t="n">
+        <v>115</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -52136,7 +52698,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -52149,8 +52711,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G96" t="inlineStr"/>
-      <c r="H96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>UHWI BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>1740-CASH</t>
+        </is>
+      </c>
       <c r="I96" t="inlineStr">
         <is>
           <t>11</t>
@@ -52190,7 +52760,7 @@
       </c>
       <c r="X96" t="inlineStr">
         <is>
-          <t>CASH SHORTAGE/OVERAGE</t>
+          <t>CASH SHORTAGE</t>
         </is>
       </c>
       <c r="Y96" t="n">
@@ -52634,10 +53204,8 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="A97" t="n">
+        <v>115</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -52645,7 +53213,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>555185</v>
+        <v>536924</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -52658,8 +53226,16 @@
           <t>LODG</t>
         </is>
       </c>
-      <c r="G97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>UHWI BANK 01.05.2024</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
       <c r="I97" t="inlineStr">
         <is>
           <t>11</t>

</xml_diff>

<commit_message>
Assign DEBITAMT and CREDITAMT on Batch_Detail based on positive/negative DTLAMOUNT
</commit_message>
<xml_diff>
--- a/CASH REPORT.xlsx
+++ b/CASH REPORT.xlsx
@@ -1341,7 +1341,7 @@
         <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1861,7 +1861,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2381,7 +2381,7 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2901,7 +2901,7 @@
         <v>115</v>
       </c>
       <c r="B5" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -4288,7 +4288,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -4373,7 +4373,9 @@
       <c r="AF2" t="n">
         <v>553147.46</v>
       </c>
-      <c r="AG2" t="inlineStr"/>
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
       <c r="AH2" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -4803,7 +4805,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -4888,7 +4890,9 @@
       <c r="AF3" t="n">
         <v>0</v>
       </c>
-      <c r="AG3" t="inlineStr"/>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
       <c r="AH3" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -5318,7 +5322,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -5403,7 +5407,9 @@
       <c r="AF4" t="n">
         <v>0</v>
       </c>
-      <c r="AG4" t="inlineStr"/>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
       <c r="AH4" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -5833,7 +5839,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -5918,7 +5924,9 @@
       <c r="AF5" t="n">
         <v>0</v>
       </c>
-      <c r="AG5" t="inlineStr"/>
+      <c r="AG5" t="n">
+        <v>0</v>
+      </c>
       <c r="AH5" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -6348,7 +6356,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6433,7 +6441,9 @@
       <c r="AF6" t="n">
         <v>149332.12</v>
       </c>
-      <c r="AG6" t="inlineStr"/>
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
       <c r="AH6" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -6863,7 +6873,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -6948,7 +6958,9 @@
       <c r="AF7" t="n">
         <v>66558.37</v>
       </c>
-      <c r="AG7" t="inlineStr"/>
+      <c r="AG7" t="n">
+        <v>0</v>
+      </c>
       <c r="AH7" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -7378,7 +7390,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -7461,9 +7473,11 @@
         </is>
       </c>
       <c r="AF8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG8" t="n">
         <v>-553147.46</v>
       </c>
-      <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -7893,7 +7907,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -7978,7 +7992,9 @@
       <c r="AF9" t="n">
         <v>0</v>
       </c>
-      <c r="AG9" t="inlineStr"/>
+      <c r="AG9" t="n">
+        <v>0</v>
+      </c>
       <c r="AH9" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -8408,7 +8424,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -8493,7 +8509,9 @@
       <c r="AF10" t="n">
         <v>448477.56</v>
       </c>
-      <c r="AG10" t="inlineStr"/>
+      <c r="AG10" t="n">
+        <v>0</v>
+      </c>
       <c r="AH10" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -8923,7 +8941,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -9008,7 +9026,9 @@
       <c r="AF11" t="n">
         <v>12806.96</v>
       </c>
-      <c r="AG11" t="inlineStr"/>
+      <c r="AG11" t="n">
+        <v>0</v>
+      </c>
       <c r="AH11" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -9438,7 +9458,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -9523,7 +9543,9 @@
       <c r="AF12" t="n">
         <v>0</v>
       </c>
-      <c r="AG12" t="inlineStr"/>
+      <c r="AG12" t="n">
+        <v>0</v>
+      </c>
       <c r="AH12" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -9953,7 +9975,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -10038,7 +10060,9 @@
       <c r="AF13" t="n">
         <v>0</v>
       </c>
-      <c r="AG13" t="inlineStr"/>
+      <c r="AG13" t="n">
+        <v>0</v>
+      </c>
       <c r="AH13" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -10468,7 +10492,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -10553,7 +10577,9 @@
       <c r="AF14" t="n">
         <v>131694.15</v>
       </c>
-      <c r="AG14" t="inlineStr"/>
+      <c r="AG14" t="n">
+        <v>0</v>
+      </c>
       <c r="AH14" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -10983,7 +11009,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -11068,7 +11094,9 @@
       <c r="AF15" t="n">
         <v>195815.86</v>
       </c>
-      <c r="AG15" t="inlineStr"/>
+      <c r="AG15" t="n">
+        <v>0</v>
+      </c>
       <c r="AH15" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -11498,7 +11526,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -11581,9 +11609,11 @@
         </is>
       </c>
       <c r="AF16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG16" t="n">
         <v>-2898.56</v>
       </c>
-      <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -12013,7 +12043,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -12098,7 +12128,9 @@
       <c r="AF17" t="n">
         <v>0</v>
       </c>
-      <c r="AG17" t="inlineStr"/>
+      <c r="AG17" t="n">
+        <v>0</v>
+      </c>
       <c r="AH17" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -12528,7 +12560,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -12613,7 +12645,9 @@
       <c r="AF18" t="n">
         <v>275606.79</v>
       </c>
-      <c r="AG18" t="inlineStr"/>
+      <c r="AG18" t="n">
+        <v>0</v>
+      </c>
       <c r="AH18" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -13043,7 +13077,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -13128,7 +13162,9 @@
       <c r="AF19" t="n">
         <v>0</v>
       </c>
-      <c r="AG19" t="inlineStr"/>
+      <c r="AG19" t="n">
+        <v>0</v>
+      </c>
       <c r="AH19" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -13558,7 +13594,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -13643,7 +13679,9 @@
       <c r="AF20" t="n">
         <v>0</v>
       </c>
-      <c r="AG20" t="inlineStr"/>
+      <c r="AG20" t="n">
+        <v>0</v>
+      </c>
       <c r="AH20" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -14073,7 +14111,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -14158,7 +14196,9 @@
       <c r="AF21" t="n">
         <v>0</v>
       </c>
-      <c r="AG21" t="inlineStr"/>
+      <c r="AG21" t="n">
+        <v>0</v>
+      </c>
       <c r="AH21" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -14588,7 +14628,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -14673,7 +14713,9 @@
       <c r="AF22" t="n">
         <v>323119.64</v>
       </c>
-      <c r="AG22" t="inlineStr"/>
+      <c r="AG22" t="n">
+        <v>0</v>
+      </c>
       <c r="AH22" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -15103,7 +15145,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -15188,7 +15230,9 @@
       <c r="AF23" t="n">
         <v>0</v>
       </c>
-      <c r="AG23" t="inlineStr"/>
+      <c r="AG23" t="n">
+        <v>0</v>
+      </c>
       <c r="AH23" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -15618,7 +15662,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -15701,9 +15745,11 @@
         </is>
       </c>
       <c r="AF24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG24" t="n">
         <v>-275606.79</v>
       </c>
-      <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -16133,7 +16179,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -16218,7 +16264,9 @@
       <c r="AF25" t="n">
         <v>2700</v>
       </c>
-      <c r="AG25" t="inlineStr"/>
+      <c r="AG25" t="n">
+        <v>0</v>
+      </c>
       <c r="AH25" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -16648,7 +16696,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -16733,7 +16781,9 @@
       <c r="AF26" t="n">
         <v>65195.99</v>
       </c>
-      <c r="AG26" t="inlineStr"/>
+      <c r="AG26" t="n">
+        <v>0</v>
+      </c>
       <c r="AH26" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -17163,7 +17213,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -17248,7 +17298,9 @@
       <c r="AF27" t="n">
         <v>0</v>
       </c>
-      <c r="AG27" t="inlineStr"/>
+      <c r="AG27" t="n">
+        <v>0</v>
+      </c>
       <c r="AH27" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -17678,7 +17730,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -17763,7 +17815,9 @@
       <c r="AF28" t="n">
         <v>0</v>
       </c>
-      <c r="AG28" t="inlineStr"/>
+      <c r="AG28" t="n">
+        <v>0</v>
+      </c>
       <c r="AH28" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -18193,7 +18247,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -18278,7 +18332,9 @@
       <c r="AF29" t="n">
         <v>0</v>
       </c>
-      <c r="AG29" t="inlineStr"/>
+      <c r="AG29" t="n">
+        <v>0</v>
+      </c>
       <c r="AH29" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -18708,7 +18764,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -18793,7 +18849,9 @@
       <c r="AF30" t="n">
         <v>39120.04</v>
       </c>
-      <c r="AG30" t="inlineStr"/>
+      <c r="AG30" t="n">
+        <v>0</v>
+      </c>
       <c r="AH30" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -19223,7 +19281,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -19308,7 +19366,9 @@
       <c r="AF31" t="n">
         <v>0</v>
       </c>
-      <c r="AG31" t="inlineStr"/>
+      <c r="AG31" t="n">
+        <v>0</v>
+      </c>
       <c r="AH31" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -19738,7 +19798,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -19821,9 +19881,11 @@
         </is>
       </c>
       <c r="AF32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG32" t="n">
         <v>-65195.99</v>
       </c>
-      <c r="AG32" t="inlineStr"/>
       <c r="AH32" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -20253,7 +20315,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -20338,7 +20400,9 @@
       <c r="AF33" t="n">
         <v>0</v>
       </c>
-      <c r="AG33" t="inlineStr"/>
+      <c r="AG33" t="n">
+        <v>0</v>
+      </c>
       <c r="AH33" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -20768,7 +20832,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -20853,7 +20917,9 @@
       <c r="AF34" t="n">
         <v>379541.77</v>
       </c>
-      <c r="AG34" t="inlineStr"/>
+      <c r="AG34" t="n">
+        <v>0</v>
+      </c>
       <c r="AH34" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -21283,7 +21349,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -21368,7 +21434,9 @@
       <c r="AF35" t="n">
         <v>0</v>
       </c>
-      <c r="AG35" t="inlineStr"/>
+      <c r="AG35" t="n">
+        <v>0</v>
+      </c>
       <c r="AH35" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -21798,7 +21866,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -21883,7 +21951,9 @@
       <c r="AF36" t="n">
         <v>0</v>
       </c>
-      <c r="AG36" t="inlineStr"/>
+      <c r="AG36" t="n">
+        <v>0</v>
+      </c>
       <c r="AH36" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -22313,7 +22383,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -22398,7 +22468,9 @@
       <c r="AF37" t="n">
         <v>0</v>
       </c>
-      <c r="AG37" t="inlineStr"/>
+      <c r="AG37" t="n">
+        <v>0</v>
+      </c>
       <c r="AH37" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -22828,7 +22900,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -22913,7 +22985,9 @@
       <c r="AF38" t="n">
         <v>109195.08</v>
       </c>
-      <c r="AG38" t="inlineStr"/>
+      <c r="AG38" t="n">
+        <v>0</v>
+      </c>
       <c r="AH38" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -23343,7 +23417,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -23428,7 +23502,9 @@
       <c r="AF39" t="n">
         <v>0</v>
       </c>
-      <c r="AG39" t="inlineStr"/>
+      <c r="AG39" t="n">
+        <v>0</v>
+      </c>
       <c r="AH39" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -23858,7 +23934,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -23941,9 +24017,11 @@
         </is>
       </c>
       <c r="AF40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG40" t="n">
         <v>-379541.77</v>
       </c>
-      <c r="AG40" t="inlineStr"/>
       <c r="AH40" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -24373,7 +24451,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -24458,7 +24536,9 @@
       <c r="AF41" t="n">
         <v>0</v>
       </c>
-      <c r="AG41" t="inlineStr"/>
+      <c r="AG41" t="n">
+        <v>0</v>
+      </c>
       <c r="AH41" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -24888,7 +24968,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -24973,7 +25053,9 @@
       <c r="AF42" t="n">
         <v>505116.46</v>
       </c>
-      <c r="AG42" t="inlineStr"/>
+      <c r="AG42" t="n">
+        <v>0</v>
+      </c>
       <c r="AH42" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -25403,7 +25485,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -25488,7 +25570,9 @@
       <c r="AF43" t="n">
         <v>0</v>
       </c>
-      <c r="AG43" t="inlineStr"/>
+      <c r="AG43" t="n">
+        <v>0</v>
+      </c>
       <c r="AH43" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -25918,7 +26002,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -26003,7 +26087,9 @@
       <c r="AF44" t="n">
         <v>0</v>
       </c>
-      <c r="AG44" t="inlineStr"/>
+      <c r="AG44" t="n">
+        <v>0</v>
+      </c>
       <c r="AH44" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -26433,7 +26519,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -26518,7 +26604,9 @@
       <c r="AF45" t="n">
         <v>0</v>
       </c>
-      <c r="AG45" t="inlineStr"/>
+      <c r="AG45" t="n">
+        <v>0</v>
+      </c>
       <c r="AH45" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -26948,7 +27036,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -27033,7 +27121,9 @@
       <c r="AF46" t="n">
         <v>92425.00999999999</v>
       </c>
-      <c r="AG46" t="inlineStr"/>
+      <c r="AG46" t="n">
+        <v>0</v>
+      </c>
       <c r="AH46" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -27463,7 +27553,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -27548,7 +27638,9 @@
       <c r="AF47" t="n">
         <v>26099.94</v>
       </c>
-      <c r="AG47" t="inlineStr"/>
+      <c r="AG47" t="n">
+        <v>0</v>
+      </c>
       <c r="AH47" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -27978,7 +28070,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -28061,9 +28153,11 @@
         </is>
       </c>
       <c r="AF48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG48" t="n">
         <v>-505116.46</v>
       </c>
-      <c r="AG48" t="inlineStr"/>
       <c r="AH48" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -28493,7 +28587,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -28578,7 +28672,9 @@
       <c r="AF49" t="n">
         <v>0</v>
       </c>
-      <c r="AG49" t="inlineStr"/>
+      <c r="AG49" t="n">
+        <v>0</v>
+      </c>
       <c r="AH49" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -29008,7 +29104,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -29093,7 +29189,9 @@
       <c r="AF50" t="n">
         <v>0</v>
       </c>
-      <c r="AG50" t="inlineStr"/>
+      <c r="AG50" t="n">
+        <v>0</v>
+      </c>
       <c r="AH50" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -29523,7 +29621,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -29608,7 +29706,9 @@
       <c r="AF51" t="n">
         <v>0</v>
       </c>
-      <c r="AG51" t="inlineStr"/>
+      <c r="AG51" t="n">
+        <v>0</v>
+      </c>
       <c r="AH51" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -30038,7 +30138,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -30123,7 +30223,9 @@
       <c r="AF52" t="n">
         <v>0</v>
       </c>
-      <c r="AG52" t="inlineStr"/>
+      <c r="AG52" t="n">
+        <v>0</v>
+      </c>
       <c r="AH52" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -30553,7 +30655,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -30638,7 +30740,9 @@
       <c r="AF53" t="n">
         <v>0</v>
       </c>
-      <c r="AG53" t="inlineStr"/>
+      <c r="AG53" t="n">
+        <v>0</v>
+      </c>
       <c r="AH53" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -31068,7 +31172,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -31153,7 +31257,9 @@
       <c r="AF54" t="n">
         <v>0</v>
       </c>
-      <c r="AG54" t="inlineStr"/>
+      <c r="AG54" t="n">
+        <v>0</v>
+      </c>
       <c r="AH54" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -31583,7 +31689,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -31668,7 +31774,9 @@
       <c r="AF55" t="n">
         <v>0</v>
       </c>
-      <c r="AG55" t="inlineStr"/>
+      <c r="AG55" t="n">
+        <v>0</v>
+      </c>
       <c r="AH55" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -32098,7 +32206,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -32183,7 +32291,9 @@
       <c r="AF56" t="n">
         <v>0</v>
       </c>
-      <c r="AG56" t="inlineStr"/>
+      <c r="AG56" t="n">
+        <v>0</v>
+      </c>
       <c r="AH56" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -32613,7 +32723,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -32698,7 +32808,9 @@
       <c r="AF57" t="n">
         <v>0</v>
       </c>
-      <c r="AG57" t="inlineStr"/>
+      <c r="AG57" t="n">
+        <v>0</v>
+      </c>
       <c r="AH57" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -33128,7 +33240,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -33213,7 +33325,9 @@
       <c r="AF58" t="n">
         <v>203471.24</v>
       </c>
-      <c r="AG58" t="inlineStr"/>
+      <c r="AG58" t="n">
+        <v>0</v>
+      </c>
       <c r="AH58" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -33643,7 +33757,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -33728,7 +33842,9 @@
       <c r="AF59" t="n">
         <v>0</v>
       </c>
-      <c r="AG59" t="inlineStr"/>
+      <c r="AG59" t="n">
+        <v>0</v>
+      </c>
       <c r="AH59" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -34158,7 +34274,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -34243,7 +34359,9 @@
       <c r="AF60" t="n">
         <v>0</v>
       </c>
-      <c r="AG60" t="inlineStr"/>
+      <c r="AG60" t="n">
+        <v>0</v>
+      </c>
       <c r="AH60" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -34673,7 +34791,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -34758,7 +34876,9 @@
       <c r="AF61" t="n">
         <v>0</v>
       </c>
-      <c r="AG61" t="inlineStr"/>
+      <c r="AG61" t="n">
+        <v>0</v>
+      </c>
       <c r="AH61" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -35188,7 +35308,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -35273,7 +35393,9 @@
       <c r="AF62" t="n">
         <v>38065.02</v>
       </c>
-      <c r="AG62" t="inlineStr"/>
+      <c r="AG62" t="n">
+        <v>0</v>
+      </c>
       <c r="AH62" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -35703,7 +35825,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -35788,7 +35910,9 @@
       <c r="AF63" t="n">
         <v>0</v>
       </c>
-      <c r="AG63" t="inlineStr"/>
+      <c r="AG63" t="n">
+        <v>0</v>
+      </c>
       <c r="AH63" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -36218,7 +36342,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -36303,7 +36427,9 @@
       <c r="AF64" t="n">
         <v>8.76</v>
       </c>
-      <c r="AG64" t="inlineStr"/>
+      <c r="AG64" t="n">
+        <v>0</v>
+      </c>
       <c r="AH64" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -36733,7 +36859,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -36818,7 +36944,9 @@
       <c r="AF65" t="n">
         <v>0</v>
       </c>
-      <c r="AG65" t="inlineStr"/>
+      <c r="AG65" t="n">
+        <v>0</v>
+      </c>
       <c r="AH65" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -37248,7 +37376,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -37333,7 +37461,9 @@
       <c r="AF66" t="n">
         <v>821534.9300000001</v>
       </c>
-      <c r="AG66" t="inlineStr"/>
+      <c r="AG66" t="n">
+        <v>0</v>
+      </c>
       <c r="AH66" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -37763,7 +37893,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -37848,7 +37978,9 @@
       <c r="AF67" t="n">
         <v>0</v>
       </c>
-      <c r="AG67" t="inlineStr"/>
+      <c r="AG67" t="n">
+        <v>0</v>
+      </c>
       <c r="AH67" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -38278,7 +38410,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -38363,7 +38495,9 @@
       <c r="AF68" t="n">
         <v>0</v>
       </c>
-      <c r="AG68" t="inlineStr"/>
+      <c r="AG68" t="n">
+        <v>0</v>
+      </c>
       <c r="AH68" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -38793,7 +38927,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -38878,7 +39012,9 @@
       <c r="AF69" t="n">
         <v>0</v>
       </c>
-      <c r="AG69" t="inlineStr"/>
+      <c r="AG69" t="n">
+        <v>0</v>
+      </c>
       <c r="AH69" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -39308,7 +39444,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -39393,7 +39529,9 @@
       <c r="AF70" t="n">
         <v>105292.04</v>
       </c>
-      <c r="AG70" t="inlineStr"/>
+      <c r="AG70" t="n">
+        <v>0</v>
+      </c>
       <c r="AH70" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -39823,7 +39961,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -39908,7 +40046,9 @@
       <c r="AF71" t="n">
         <v>146284.53</v>
       </c>
-      <c r="AG71" t="inlineStr"/>
+      <c r="AG71" t="n">
+        <v>0</v>
+      </c>
       <c r="AH71" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -40338,7 +40478,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -40421,9 +40561,11 @@
         </is>
       </c>
       <c r="AF72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG72" t="n">
         <v>-821534.9300000001</v>
       </c>
-      <c r="AG72" t="inlineStr"/>
       <c r="AH72" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -40853,7 +40995,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -40938,7 +41080,9 @@
       <c r="AF73" t="n">
         <v>16605</v>
       </c>
-      <c r="AG73" t="inlineStr"/>
+      <c r="AG73" t="n">
+        <v>0</v>
+      </c>
       <c r="AH73" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -41368,7 +41512,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -41453,7 +41597,9 @@
       <c r="AF74" t="n">
         <v>400338.7</v>
       </c>
-      <c r="AG74" t="inlineStr"/>
+      <c r="AG74" t="n">
+        <v>0</v>
+      </c>
       <c r="AH74" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -41883,7 +42029,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -41968,7 +42114,9 @@
       <c r="AF75" t="n">
         <v>0</v>
       </c>
-      <c r="AG75" t="inlineStr"/>
+      <c r="AG75" t="n">
+        <v>0</v>
+      </c>
       <c r="AH75" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -42398,7 +42546,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -42483,7 +42631,9 @@
       <c r="AF76" t="n">
         <v>0</v>
       </c>
-      <c r="AG76" t="inlineStr"/>
+      <c r="AG76" t="n">
+        <v>0</v>
+      </c>
       <c r="AH76" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -42913,7 +43063,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -42998,7 +43148,9 @@
       <c r="AF77" t="n">
         <v>0</v>
       </c>
-      <c r="AG77" t="inlineStr"/>
+      <c r="AG77" t="n">
+        <v>0</v>
+      </c>
       <c r="AH77" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -43428,7 +43580,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -43513,7 +43665,9 @@
       <c r="AF78" t="n">
         <v>47365.71</v>
       </c>
-      <c r="AG78" t="inlineStr"/>
+      <c r="AG78" t="n">
+        <v>0</v>
+      </c>
       <c r="AH78" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -43943,7 +44097,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -44028,7 +44182,9 @@
       <c r="AF79" t="n">
         <v>60470.91</v>
       </c>
-      <c r="AG79" t="inlineStr"/>
+      <c r="AG79" t="n">
+        <v>0</v>
+      </c>
       <c r="AH79" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -44458,7 +44614,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -44543,7 +44699,9 @@
       <c r="AF80" t="n">
         <v>286.3</v>
       </c>
-      <c r="AG80" t="inlineStr"/>
+      <c r="AG80" t="n">
+        <v>0</v>
+      </c>
       <c r="AH80" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -44973,7 +45131,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -45058,7 +45216,9 @@
       <c r="AF81" t="n">
         <v>0</v>
       </c>
-      <c r="AG81" t="inlineStr"/>
+      <c r="AG81" t="n">
+        <v>0</v>
+      </c>
       <c r="AH81" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -45488,7 +45648,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -45573,7 +45733,9 @@
       <c r="AF82" t="n">
         <v>328243.51</v>
       </c>
-      <c r="AG82" t="inlineStr"/>
+      <c r="AG82" t="n">
+        <v>0</v>
+      </c>
       <c r="AH82" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -46003,7 +46165,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -46088,7 +46250,9 @@
       <c r="AF83" t="n">
         <v>0</v>
       </c>
-      <c r="AG83" t="inlineStr"/>
+      <c r="AG83" t="n">
+        <v>0</v>
+      </c>
       <c r="AH83" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -46518,7 +46682,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -46603,7 +46767,9 @@
       <c r="AF84" t="n">
         <v>0</v>
       </c>
-      <c r="AG84" t="inlineStr"/>
+      <c r="AG84" t="n">
+        <v>0</v>
+      </c>
       <c r="AH84" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -47033,7 +47199,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -47118,7 +47284,9 @@
       <c r="AF85" t="n">
         <v>0</v>
       </c>
-      <c r="AG85" t="inlineStr"/>
+      <c r="AG85" t="n">
+        <v>0</v>
+      </c>
       <c r="AH85" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -47548,7 +47716,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -47633,7 +47801,9 @@
       <c r="AF86" t="n">
         <v>29200.08</v>
       </c>
-      <c r="AG86" t="inlineStr"/>
+      <c r="AG86" t="n">
+        <v>0</v>
+      </c>
       <c r="AH86" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -48063,7 +48233,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -48148,7 +48318,9 @@
       <c r="AF87" t="n">
         <v>0</v>
       </c>
-      <c r="AG87" t="inlineStr"/>
+      <c r="AG87" t="n">
+        <v>0</v>
+      </c>
       <c r="AH87" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -48578,7 +48750,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -48661,9 +48833,11 @@
         </is>
       </c>
       <c r="AF88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG88" t="n">
         <v>-328243.51</v>
       </c>
-      <c r="AG88" t="inlineStr"/>
       <c r="AH88" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -49093,7 +49267,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -49178,7 +49352,9 @@
       <c r="AF89" t="n">
         <v>0</v>
       </c>
-      <c r="AG89" t="inlineStr"/>
+      <c r="AG89" t="n">
+        <v>0</v>
+      </c>
       <c r="AH89" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -49608,7 +49784,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -49693,7 +49869,9 @@
       <c r="AF90" t="n">
         <v>364073.99</v>
       </c>
-      <c r="AG90" t="inlineStr"/>
+      <c r="AG90" t="n">
+        <v>0</v>
+      </c>
       <c r="AH90" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -50123,7 +50301,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -50208,7 +50386,9 @@
       <c r="AF91" t="n">
         <v>0</v>
       </c>
-      <c r="AG91" t="inlineStr"/>
+      <c r="AG91" t="n">
+        <v>0</v>
+      </c>
       <c r="AH91" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -50638,7 +50818,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -50723,7 +50903,9 @@
       <c r="AF92" t="n">
         <v>0</v>
       </c>
-      <c r="AG92" t="inlineStr"/>
+      <c r="AG92" t="n">
+        <v>0</v>
+      </c>
       <c r="AH92" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -51153,7 +51335,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -51238,7 +51420,9 @@
       <c r="AF93" t="n">
         <v>0</v>
       </c>
-      <c r="AG93" t="inlineStr"/>
+      <c r="AG93" t="n">
+        <v>0</v>
+      </c>
       <c r="AH93" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -51668,7 +51852,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -51753,7 +51937,9 @@
       <c r="AF94" t="n">
         <v>304804.33</v>
       </c>
-      <c r="AG94" t="inlineStr"/>
+      <c r="AG94" t="n">
+        <v>0</v>
+      </c>
       <c r="AH94" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -52183,7 +52369,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -52268,7 +52454,9 @@
       <c r="AF95" t="n">
         <v>0</v>
       </c>
-      <c r="AG95" t="inlineStr"/>
+      <c r="AG95" t="n">
+        <v>0</v>
+      </c>
       <c r="AH95" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -52698,7 +52886,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -52781,9 +52969,11 @@
         </is>
       </c>
       <c r="AF96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG96" t="n">
         <v>-2558.99</v>
       </c>
-      <c r="AG96" t="inlineStr"/>
       <c r="AH96" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -53213,7 +53403,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>536924</v>
+        <v>825001</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -53298,7 +53488,9 @@
       <c r="AF97" t="n">
         <v>0</v>
       </c>
-      <c r="AG97" t="inlineStr"/>
+      <c r="AG97" t="n">
+        <v>0</v>
+      </c>
       <c r="AH97" t="inlineStr">
         <is>
           <t>FALSE</t>

</xml_diff>

<commit_message>
Assign NODETAILS based on count of matching Batch Detail records on ENTRYNO
</commit_message>
<xml_diff>
--- a/CASH REPORT.xlsx
+++ b/CASH REPORT.xlsx
@@ -1341,7 +1341,7 @@
         <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1387,7 +1387,9 @@
       <c r="N2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="O2" t="n">
+        <v>8</v>
+      </c>
       <c r="P2" t="n">
         <v>445579</v>
       </c>
@@ -1861,7 +1863,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1907,7 +1909,9 @@
       <c r="N3" t="n">
         <v>0</v>
       </c>
-      <c r="O3" t="inlineStr"/>
+      <c r="O3" t="n">
+        <v>8</v>
+      </c>
       <c r="P3" t="n">
         <v>203480</v>
       </c>
@@ -2381,7 +2385,7 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2427,7 +2431,9 @@
       <c r="N4" t="n">
         <v>0</v>
       </c>
-      <c r="O4" t="inlineStr"/>
+      <c r="O4" t="n">
+        <v>8</v>
+      </c>
       <c r="P4" t="n">
         <v>400625</v>
       </c>
@@ -2901,7 +2907,7 @@
         <v>115</v>
       </c>
       <c r="B5" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -2947,7 +2953,9 @@
       <c r="N5" t="n">
         <v>0</v>
       </c>
-      <c r="O5" t="inlineStr"/>
+      <c r="O5" t="n">
+        <v>8</v>
+      </c>
       <c r="P5" t="n">
         <v>361515</v>
       </c>
@@ -4288,7 +4296,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -4805,7 +4813,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -5322,7 +5330,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -5839,7 +5847,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6356,7 +6364,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6873,7 +6881,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -7390,7 +7398,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -7907,7 +7915,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -8424,7 +8432,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -8941,7 +8949,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -9458,7 +9466,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -9975,7 +9983,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -10492,7 +10500,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -11009,7 +11017,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -11526,7 +11534,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -12043,7 +12051,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -12560,7 +12568,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -13077,7 +13085,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -13594,7 +13602,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -14111,7 +14119,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -14628,7 +14636,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -15145,7 +15153,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -15662,7 +15670,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -16179,7 +16187,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -16696,7 +16704,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -17213,7 +17221,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -17730,7 +17738,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -18247,7 +18255,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -18764,7 +18772,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -19281,7 +19289,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -19798,7 +19806,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -20315,7 +20323,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -20832,7 +20840,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -21349,7 +21357,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -21866,7 +21874,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -22383,7 +22391,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -22900,7 +22908,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -23417,7 +23425,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -23934,7 +23942,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -24451,7 +24459,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -24968,7 +24976,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -25485,7 +25493,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -26002,7 +26010,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -26519,7 +26527,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -27036,7 +27044,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -27553,7 +27561,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -28070,7 +28078,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -28587,7 +28595,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -29104,7 +29112,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -29621,7 +29629,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -30138,7 +30146,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -30655,7 +30663,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -31172,7 +31180,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -31689,7 +31697,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -32206,7 +32214,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -32723,7 +32731,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -33240,7 +33248,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -33757,7 +33765,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -34274,7 +34282,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -34791,7 +34799,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -35308,7 +35316,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -35825,7 +35833,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -36342,7 +36350,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -36859,7 +36867,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -37376,7 +37384,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -37893,7 +37901,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -38410,7 +38418,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -38927,7 +38935,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -39444,7 +39452,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -39961,7 +39969,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -40478,7 +40486,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -40995,7 +41003,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -41512,7 +41520,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -42029,7 +42037,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -42546,7 +42554,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -43063,7 +43071,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -43580,7 +43588,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -44097,7 +44105,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -44614,7 +44622,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -45131,7 +45139,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -45648,7 +45656,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -46165,7 +46173,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -46682,7 +46690,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -47199,7 +47207,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -47716,7 +47724,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -48233,7 +48241,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -48750,7 +48758,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -49267,7 +49275,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -49784,7 +49792,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -50301,7 +50309,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -50818,7 +50826,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -51335,7 +51343,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -51852,7 +51860,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -52369,7 +52377,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -52886,7 +52894,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -53403,7 +53411,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>825001</v>
+        <v>274781</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Create Batch_Miscellaneous sheet  * Create Batch_Miscellaneous DataFrame as subset of Batch Header DataFrame  * Add columns from Batch_Miscellaneous DataFrame2 to Batch_Miscellaneous DataFrame  * Set Defaults for some columns on Batch_Miscellaneous DataFrame
</commit_message>
<xml_diff>
--- a/CASH REPORT.xlsx
+++ b/CASH REPORT.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Batch_Header" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Batch_Detail" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Batch_Miscellaneous" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1341,7 +1342,7 @@
         <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1863,7 +1864,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2385,7 +2386,7 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2907,7 +2908,7 @@
         <v>115</v>
       </c>
       <c r="B5" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -4296,7 +4297,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -4813,7 +4814,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -5330,7 +5331,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -5847,7 +5848,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6364,7 +6365,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6881,7 +6882,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -7398,7 +7399,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -7915,7 +7916,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -8432,7 +8433,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -8949,7 +8950,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -9466,7 +9467,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -9983,7 +9984,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -10500,7 +10501,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -11017,7 +11018,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -11534,7 +11535,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -12051,7 +12052,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -12568,7 +12569,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -13085,7 +13086,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -13602,7 +13603,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -14119,7 +14120,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -14636,7 +14637,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -15153,7 +15154,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -15670,7 +15671,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -16187,7 +16188,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -16704,7 +16705,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -17221,7 +17222,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -17738,7 +17739,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -18255,7 +18256,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -18772,7 +18773,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -19289,7 +19290,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -19806,7 +19807,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -20323,7 +20324,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -20840,7 +20841,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -21357,7 +21358,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -21874,7 +21875,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -22391,7 +22392,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -22908,7 +22909,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -23425,7 +23426,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -23942,7 +23943,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -24459,7 +24460,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -24976,7 +24977,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -25493,7 +25494,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -26010,7 +26011,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -26527,7 +26528,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -27044,7 +27045,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -27561,7 +27562,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -28078,7 +28079,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -28595,7 +28596,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -29112,7 +29113,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -29629,7 +29630,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -30146,7 +30147,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -30663,7 +30664,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -31180,7 +31181,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -31697,7 +31698,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -32214,7 +32215,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -32731,7 +32732,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -33248,7 +33249,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -33765,7 +33766,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -34282,7 +34283,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -34799,7 +34800,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -35316,7 +35317,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -35833,7 +35834,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -36350,7 +36351,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -36867,7 +36868,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -37384,7 +37385,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -37901,7 +37902,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -38418,7 +38419,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -38935,7 +38936,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -39452,7 +39453,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -39969,7 +39970,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -40486,7 +40487,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -41003,7 +41004,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -41520,7 +41521,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -42037,7 +42038,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -42554,7 +42555,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -43071,7 +43072,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -43588,7 +43589,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -44105,7 +44106,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -44622,7 +44623,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -45139,7 +45140,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -45656,7 +45657,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -46173,7 +46174,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -46690,7 +46691,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -47207,7 +47208,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -47724,7 +47725,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -48241,7 +48242,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -48758,7 +48759,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -49275,7 +49276,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -49792,7 +49793,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -50309,7 +50310,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -50826,7 +50827,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -51343,7 +51344,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -51860,7 +51861,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -52377,7 +52378,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -52894,7 +52895,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -53411,7 +53412,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>274781</v>
+        <v>915726</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -53917,6 +53918,535 @@
           <t>FALSE</t>
         </is>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AR5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>BATCHID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ENTRYNO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DETAILNO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>MISCCODE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>NAME</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ADDRESS1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ADDRESS2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ADDRESS3</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ADDRESS4</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>POSTCODE</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>PHONE1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>PHONE2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>FAXNUMBER</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>CONTACT</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>COMMENTS</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>SWKEEPTOT</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>ACCTROW</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>ACCTNAME</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>ACCTNO</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>CITY</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>COUNTRY</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>EMAILADDR</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>URLADDR</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>SWAPPROVED</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>EFTDESC</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>BANKNAME</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>ACCOUNT</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>BRANCH</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>ACCTYPE</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>BANKID</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>SWIFTCTY</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>PAYDETL</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>ADDINFO1</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>ADDINFO2</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>COVERTYPE</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>COVERINFO</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>BENCODE</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>EITYPE</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>BOPCATG</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>BOPREF</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>BOPDESC</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>BRN</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>IDN</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>915726</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>00001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0000000200</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>915726</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>00002</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0000000200</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>915726</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>00003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0000000200</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>915726</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>00004</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0000000200</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Create remaining DataFrames based on CSV Templates
</commit_message>
<xml_diff>
--- a/CASH REPORT.xlsx
+++ b/CASH REPORT.xlsx
@@ -10,6 +10,10 @@
     <sheet name="Batch_Header" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Batch_Detail" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Batch_Miscellaneous" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Batch_Sub_Detail" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Batch_Detail_Adjustments" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Batch_Header_Optional_Fields" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Batch_Detail_Optional_Fields" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1342,7 +1346,7 @@
         <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1864,7 +1868,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2386,7 +2390,7 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2908,7 +2912,7 @@
         <v>115</v>
       </c>
       <c r="B5" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -4297,7 +4301,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -4814,7 +4818,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -5331,7 +5335,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -5848,7 +5852,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6365,7 +6369,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6882,7 +6886,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -7399,7 +7403,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -7916,7 +7920,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -8433,7 +8437,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -8950,7 +8954,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -9467,7 +9471,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -9984,7 +9988,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -10501,7 +10505,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -11018,7 +11022,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -11535,7 +11539,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -12052,7 +12056,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -12569,7 +12573,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -13086,7 +13090,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -13603,7 +13607,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -14120,7 +14124,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -14637,7 +14641,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -15154,7 +15158,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -15671,7 +15675,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -16188,7 +16192,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -16705,7 +16709,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -17222,7 +17226,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -17739,7 +17743,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -18256,7 +18260,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -18773,7 +18777,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -19290,7 +19294,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -19807,7 +19811,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -20324,7 +20328,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -20841,7 +20845,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -21358,7 +21362,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -21875,7 +21879,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -22392,7 +22396,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -22909,7 +22913,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -23426,7 +23430,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -23943,7 +23947,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -24460,7 +24464,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -24977,7 +24981,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -25494,7 +25498,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -26011,7 +26015,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -26528,7 +26532,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -27045,7 +27049,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -27562,7 +27566,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -28079,7 +28083,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -28596,7 +28600,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -29113,7 +29117,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -29630,7 +29634,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -30147,7 +30151,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -30664,7 +30668,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -31181,7 +31185,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -31698,7 +31702,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -32215,7 +32219,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -32732,7 +32736,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -33249,7 +33253,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -33766,7 +33770,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -34283,7 +34287,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -34800,7 +34804,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -35317,7 +35321,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -35834,7 +35838,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -36351,7 +36355,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -36868,7 +36872,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -37385,7 +37389,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -37902,7 +37906,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -38419,7 +38423,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -38936,7 +38940,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -39453,7 +39457,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -39970,7 +39974,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -40487,7 +40491,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -41004,7 +41008,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -41521,7 +41525,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -42038,7 +42042,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -42555,7 +42559,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -43072,7 +43076,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -43589,7 +43593,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -44106,7 +44110,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -44623,7 +44627,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -45140,7 +45144,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -45657,7 +45661,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -46174,7 +46178,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -46691,7 +46695,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -47208,7 +47212,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -47725,7 +47729,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -48242,7 +48246,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -48759,7 +48763,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -49276,7 +49280,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -49793,7 +49797,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -50310,7 +50314,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -50827,7 +50831,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -51344,7 +51348,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -51861,7 +51865,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -52378,7 +52382,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -52895,7 +52899,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -53412,7 +53416,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -54162,7 +54166,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -54234,7 +54238,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -54306,7 +54310,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -54378,7 +54382,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>915726</v>
+        <v>250080</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -54451,4 +54455,728 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BE1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>BATCHID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ENTRYNO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DETAILNO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>DOCNUMBER</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>PAYNUMBER</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>SUBDETNO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>DOCTYPE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>APPLAMOUNT</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DISCOUNT</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>DATEDOC</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>IDCUST</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>PONUMBER</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>NATCUSTID</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ADJREF</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ADJDESC</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ADJAMOUNT</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>SWJOB</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>SWPOSTED</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>PJCSDAMT</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>PJCSDDISC</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>ENTRYTYPE</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>PROCESSCMD</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>PJCUNAPAMT</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>PJCUNAPDSC</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD1TC</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD2TC</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD3TC</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD4TC</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD5TC</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD1HC</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD2HC</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD3HC</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD4HC</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD5HC</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD1BC</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD2BC</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD3BC</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD4BC</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD5BC</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHTOTBC</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD1DT</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD2DT</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD3DT</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD4DT</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHD5DT</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>CODETAX1</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>CODETAX2</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>CODETAX3</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>CODETAX4</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>CODETAX5</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>AMTWHDTOT</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>CBBTADRVH</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>CBBTADVW</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>AMTREMAIN</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>APPLYMETH</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>PNDADJAMT</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>SELECTFROM</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AD1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>BATCHID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ENTRYNO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DETAILNO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>DOCNUMBER</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>PAYNUMBER</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>TRANSTYPE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>SEQNO</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>DISTCODE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DISTAMOUNT</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ACCTID</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ACCTIDUF</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>CONTRACT</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>PROJECT</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>CATEGORY</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>RESOURCE</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>COSTCLASS</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>BILLTYPE</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>ITEMNO</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>UNITOFMEAS</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>QUANTITY</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>DATEBILL</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>BILLRATE</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>BILLCUR</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>FMTCONTNO</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>DOCLINE</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>CBBTHDRVH</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>CBBTHDVW</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>SWFROMWEB</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>AMTREMAIN</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>BATCHID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ENTRYNO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>OPTFIELD</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>TYPE</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>LENGTH</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>DECIMALS</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ALLOWNULL</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>VALIDATE</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SWSET</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>VALINDEX</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFTEXT</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFMONEY</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFNUM</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFLONG</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFBOOL</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFDATE</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFTIME</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>FDESC</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>VDESC</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>BATCHID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ENTRYNO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DETAILNO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>OPTFIELD</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>TYPE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>LENGTH</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>DECIMALS</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ALLOWNULL</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>VALIDATE</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SWSET</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>VALINDEX</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFTEXT</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFMONEY</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFNUM</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFLONG</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFBOOL</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFDATE</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>VALIFTIME</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>FDESC</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>VDESC</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Assign HDRDEBIT and HDRCREDIT on Batch Header Dataframe  * Assign Batch Header columns based on sum of DEBITAMT and CREDITAMT on Batch Detail  * Removed and Added default value on Batch Detail SQL Query where needed
</commit_message>
<xml_diff>
--- a/CASH REPORT.xlsx
+++ b/CASH REPORT.xlsx
@@ -1346,7 +1346,7 @@
         <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1560,8 +1560,12 @@
       <c r="BN2" t="n">
         <v>445579</v>
       </c>
-      <c r="BO2" t="inlineStr"/>
-      <c r="BP2" t="inlineStr"/>
+      <c r="BO2" t="n">
+        <v>769037.95</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>-553147.46</v>
+      </c>
       <c r="BQ2" t="inlineStr"/>
       <c r="BR2" t="inlineStr"/>
       <c r="BS2" t="inlineStr"/>
@@ -1868,7 +1872,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2082,8 +2086,12 @@
       <c r="BN3" t="n">
         <v>203480</v>
       </c>
-      <c r="BO3" t="inlineStr"/>
-      <c r="BP3" t="inlineStr"/>
+      <c r="BO3" t="n">
+        <v>788794.53</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>-2898.56</v>
+      </c>
       <c r="BQ3" t="inlineStr"/>
       <c r="BR3" t="inlineStr"/>
       <c r="BS3" t="inlineStr"/>
@@ -2390,7 +2398,7 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2604,8 +2612,12 @@
       <c r="BN4" t="n">
         <v>400625</v>
       </c>
-      <c r="BO4" t="inlineStr"/>
-      <c r="BP4" t="inlineStr"/>
+      <c r="BO4" t="n">
+        <v>601426.4299999999</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>-275606.79</v>
+      </c>
       <c r="BQ4" t="inlineStr"/>
       <c r="BR4" t="inlineStr"/>
       <c r="BS4" t="inlineStr"/>
@@ -2912,7 +2924,7 @@
         <v>115</v>
       </c>
       <c r="B5" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -3126,8 +3138,12 @@
       <c r="BN5" t="n">
         <v>361515</v>
       </c>
-      <c r="BO5" t="inlineStr"/>
-      <c r="BP5" t="inlineStr"/>
+      <c r="BO5" t="n">
+        <v>104316.03</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>-65195.99</v>
+      </c>
       <c r="BQ5" t="inlineStr"/>
       <c r="BR5" t="inlineStr"/>
       <c r="BS5" t="inlineStr"/>
@@ -3909,7 +3925,11 @@
           <t>NOSUBDETL</t>
         </is>
       </c>
-      <c r="CO1" s="1" t="inlineStr"/>
+      <c r="CO1" s="1" t="inlineStr">
+        <is>
+          <t>VALUES</t>
+        </is>
+      </c>
       <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>PROCESSCMD</t>
@@ -4301,7 +4321,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -4566,10 +4586,8 @@
       <c r="CN2" t="n">
         <v>0</v>
       </c>
-      <c r="CO2" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO2" t="n">
+        <v>0</v>
       </c>
       <c r="CP2" t="n">
         <v>0</v>
@@ -4818,7 +4836,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -5083,10 +5101,8 @@
       <c r="CN3" t="n">
         <v>0</v>
       </c>
-      <c r="CO3" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO3" t="n">
+        <v>0</v>
       </c>
       <c r="CP3" t="n">
         <v>0</v>
@@ -5335,7 +5351,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -5600,10 +5616,8 @@
       <c r="CN4" t="n">
         <v>0</v>
       </c>
-      <c r="CO4" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO4" t="n">
+        <v>0</v>
       </c>
       <c r="CP4" t="n">
         <v>0</v>
@@ -5852,7 +5866,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6117,10 +6131,8 @@
       <c r="CN5" t="n">
         <v>0</v>
       </c>
-      <c r="CO5" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO5" t="n">
+        <v>0</v>
       </c>
       <c r="CP5" t="n">
         <v>0</v>
@@ -6369,7 +6381,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6634,10 +6646,8 @@
       <c r="CN6" t="n">
         <v>0</v>
       </c>
-      <c r="CO6" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO6" t="n">
+        <v>0</v>
       </c>
       <c r="CP6" t="n">
         <v>0</v>
@@ -6886,7 +6896,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -7151,10 +7161,8 @@
       <c r="CN7" t="n">
         <v>0</v>
       </c>
-      <c r="CO7" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO7" t="n">
+        <v>0</v>
       </c>
       <c r="CP7" t="n">
         <v>0</v>
@@ -7403,7 +7411,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -7668,10 +7676,8 @@
       <c r="CN8" t="n">
         <v>0</v>
       </c>
-      <c r="CO8" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO8" t="n">
+        <v>0</v>
       </c>
       <c r="CP8" t="n">
         <v>0</v>
@@ -7920,7 +7926,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -8185,10 +8191,8 @@
       <c r="CN9" t="n">
         <v>0</v>
       </c>
-      <c r="CO9" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO9" t="n">
+        <v>0</v>
       </c>
       <c r="CP9" t="n">
         <v>0</v>
@@ -8437,7 +8441,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -8702,10 +8706,8 @@
       <c r="CN10" t="n">
         <v>0</v>
       </c>
-      <c r="CO10" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO10" t="n">
+        <v>0</v>
       </c>
       <c r="CP10" t="n">
         <v>0</v>
@@ -8954,7 +8956,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -9219,10 +9221,8 @@
       <c r="CN11" t="n">
         <v>0</v>
       </c>
-      <c r="CO11" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO11" t="n">
+        <v>0</v>
       </c>
       <c r="CP11" t="n">
         <v>0</v>
@@ -9471,7 +9471,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -9736,10 +9736,8 @@
       <c r="CN12" t="n">
         <v>0</v>
       </c>
-      <c r="CO12" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO12" t="n">
+        <v>0</v>
       </c>
       <c r="CP12" t="n">
         <v>0</v>
@@ -9988,7 +9986,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -10253,10 +10251,8 @@
       <c r="CN13" t="n">
         <v>0</v>
       </c>
-      <c r="CO13" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO13" t="n">
+        <v>0</v>
       </c>
       <c r="CP13" t="n">
         <v>0</v>
@@ -10505,7 +10501,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -10770,10 +10766,8 @@
       <c r="CN14" t="n">
         <v>0</v>
       </c>
-      <c r="CO14" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO14" t="n">
+        <v>0</v>
       </c>
       <c r="CP14" t="n">
         <v>0</v>
@@ -11022,7 +11016,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -11287,10 +11281,8 @@
       <c r="CN15" t="n">
         <v>0</v>
       </c>
-      <c r="CO15" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO15" t="n">
+        <v>0</v>
       </c>
       <c r="CP15" t="n">
         <v>0</v>
@@ -11539,7 +11531,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -11804,10 +11796,8 @@
       <c r="CN16" t="n">
         <v>0</v>
       </c>
-      <c r="CO16" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO16" t="n">
+        <v>0</v>
       </c>
       <c r="CP16" t="n">
         <v>0</v>
@@ -12056,7 +12046,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -12321,10 +12311,8 @@
       <c r="CN17" t="n">
         <v>0</v>
       </c>
-      <c r="CO17" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO17" t="n">
+        <v>0</v>
       </c>
       <c r="CP17" t="n">
         <v>0</v>
@@ -12573,7 +12561,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -12838,10 +12826,8 @@
       <c r="CN18" t="n">
         <v>0</v>
       </c>
-      <c r="CO18" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO18" t="n">
+        <v>0</v>
       </c>
       <c r="CP18" t="n">
         <v>0</v>
@@ -13090,7 +13076,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -13355,10 +13341,8 @@
       <c r="CN19" t="n">
         <v>0</v>
       </c>
-      <c r="CO19" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO19" t="n">
+        <v>0</v>
       </c>
       <c r="CP19" t="n">
         <v>0</v>
@@ -13607,7 +13591,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -13872,10 +13856,8 @@
       <c r="CN20" t="n">
         <v>0</v>
       </c>
-      <c r="CO20" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO20" t="n">
+        <v>0</v>
       </c>
       <c r="CP20" t="n">
         <v>0</v>
@@ -14124,7 +14106,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -14389,10 +14371,8 @@
       <c r="CN21" t="n">
         <v>0</v>
       </c>
-      <c r="CO21" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO21" t="n">
+        <v>0</v>
       </c>
       <c r="CP21" t="n">
         <v>0</v>
@@ -14641,7 +14621,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -14906,10 +14886,8 @@
       <c r="CN22" t="n">
         <v>0</v>
       </c>
-      <c r="CO22" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO22" t="n">
+        <v>0</v>
       </c>
       <c r="CP22" t="n">
         <v>0</v>
@@ -15158,7 +15136,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -15423,10 +15401,8 @@
       <c r="CN23" t="n">
         <v>0</v>
       </c>
-      <c r="CO23" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO23" t="n">
+        <v>0</v>
       </c>
       <c r="CP23" t="n">
         <v>0</v>
@@ -15675,7 +15651,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -15940,10 +15916,8 @@
       <c r="CN24" t="n">
         <v>0</v>
       </c>
-      <c r="CO24" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO24" t="n">
+        <v>0</v>
       </c>
       <c r="CP24" t="n">
         <v>0</v>
@@ -16192,7 +16166,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -16457,10 +16431,8 @@
       <c r="CN25" t="n">
         <v>0</v>
       </c>
-      <c r="CO25" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO25" t="n">
+        <v>0</v>
       </c>
       <c r="CP25" t="n">
         <v>0</v>
@@ -16709,7 +16681,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -16974,10 +16946,8 @@
       <c r="CN26" t="n">
         <v>0</v>
       </c>
-      <c r="CO26" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO26" t="n">
+        <v>0</v>
       </c>
       <c r="CP26" t="n">
         <v>0</v>
@@ -17226,7 +17196,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -17491,10 +17461,8 @@
       <c r="CN27" t="n">
         <v>0</v>
       </c>
-      <c r="CO27" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO27" t="n">
+        <v>0</v>
       </c>
       <c r="CP27" t="n">
         <v>0</v>
@@ -17743,7 +17711,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -18008,10 +17976,8 @@
       <c r="CN28" t="n">
         <v>0</v>
       </c>
-      <c r="CO28" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO28" t="n">
+        <v>0</v>
       </c>
       <c r="CP28" t="n">
         <v>0</v>
@@ -18260,7 +18226,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -18525,10 +18491,8 @@
       <c r="CN29" t="n">
         <v>0</v>
       </c>
-      <c r="CO29" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO29" t="n">
+        <v>0</v>
       </c>
       <c r="CP29" t="n">
         <v>0</v>
@@ -18777,7 +18741,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -19042,10 +19006,8 @@
       <c r="CN30" t="n">
         <v>0</v>
       </c>
-      <c r="CO30" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO30" t="n">
+        <v>0</v>
       </c>
       <c r="CP30" t="n">
         <v>0</v>
@@ -19294,7 +19256,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -19559,10 +19521,8 @@
       <c r="CN31" t="n">
         <v>0</v>
       </c>
-      <c r="CO31" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO31" t="n">
+        <v>0</v>
       </c>
       <c r="CP31" t="n">
         <v>0</v>
@@ -19811,7 +19771,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -20076,10 +20036,8 @@
       <c r="CN32" t="n">
         <v>0</v>
       </c>
-      <c r="CO32" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO32" t="n">
+        <v>0</v>
       </c>
       <c r="CP32" t="n">
         <v>0</v>
@@ -20328,7 +20286,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -20593,10 +20551,8 @@
       <c r="CN33" t="n">
         <v>0</v>
       </c>
-      <c r="CO33" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO33" t="n">
+        <v>0</v>
       </c>
       <c r="CP33" t="n">
         <v>0</v>
@@ -20845,7 +20801,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -21110,10 +21066,8 @@
       <c r="CN34" t="n">
         <v>0</v>
       </c>
-      <c r="CO34" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO34" t="n">
+        <v>0</v>
       </c>
       <c r="CP34" t="n">
         <v>0</v>
@@ -21362,7 +21316,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -21627,10 +21581,8 @@
       <c r="CN35" t="n">
         <v>0</v>
       </c>
-      <c r="CO35" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO35" t="n">
+        <v>0</v>
       </c>
       <c r="CP35" t="n">
         <v>0</v>
@@ -21879,7 +21831,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -22144,10 +22096,8 @@
       <c r="CN36" t="n">
         <v>0</v>
       </c>
-      <c r="CO36" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO36" t="n">
+        <v>0</v>
       </c>
       <c r="CP36" t="n">
         <v>0</v>
@@ -22396,7 +22346,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -22661,10 +22611,8 @@
       <c r="CN37" t="n">
         <v>0</v>
       </c>
-      <c r="CO37" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO37" t="n">
+        <v>0</v>
       </c>
       <c r="CP37" t="n">
         <v>0</v>
@@ -22913,7 +22861,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -23178,10 +23126,8 @@
       <c r="CN38" t="n">
         <v>0</v>
       </c>
-      <c r="CO38" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO38" t="n">
+        <v>0</v>
       </c>
       <c r="CP38" t="n">
         <v>0</v>
@@ -23430,7 +23376,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -23695,10 +23641,8 @@
       <c r="CN39" t="n">
         <v>0</v>
       </c>
-      <c r="CO39" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO39" t="n">
+        <v>0</v>
       </c>
       <c r="CP39" t="n">
         <v>0</v>
@@ -23947,7 +23891,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -24212,10 +24156,8 @@
       <c r="CN40" t="n">
         <v>0</v>
       </c>
-      <c r="CO40" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO40" t="n">
+        <v>0</v>
       </c>
       <c r="CP40" t="n">
         <v>0</v>
@@ -24464,7 +24406,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -24729,10 +24671,8 @@
       <c r="CN41" t="n">
         <v>0</v>
       </c>
-      <c r="CO41" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO41" t="n">
+        <v>0</v>
       </c>
       <c r="CP41" t="n">
         <v>0</v>
@@ -24981,7 +24921,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -25246,10 +25186,8 @@
       <c r="CN42" t="n">
         <v>0</v>
       </c>
-      <c r="CO42" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO42" t="n">
+        <v>0</v>
       </c>
       <c r="CP42" t="n">
         <v>0</v>
@@ -25498,7 +25436,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -25763,10 +25701,8 @@
       <c r="CN43" t="n">
         <v>0</v>
       </c>
-      <c r="CO43" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO43" t="n">
+        <v>0</v>
       </c>
       <c r="CP43" t="n">
         <v>0</v>
@@ -26015,7 +25951,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -26280,10 +26216,8 @@
       <c r="CN44" t="n">
         <v>0</v>
       </c>
-      <c r="CO44" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO44" t="n">
+        <v>0</v>
       </c>
       <c r="CP44" t="n">
         <v>0</v>
@@ -26532,7 +26466,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -26797,10 +26731,8 @@
       <c r="CN45" t="n">
         <v>0</v>
       </c>
-      <c r="CO45" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO45" t="n">
+        <v>0</v>
       </c>
       <c r="CP45" t="n">
         <v>0</v>
@@ -27049,7 +26981,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -27314,10 +27246,8 @@
       <c r="CN46" t="n">
         <v>0</v>
       </c>
-      <c r="CO46" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO46" t="n">
+        <v>0</v>
       </c>
       <c r="CP46" t="n">
         <v>0</v>
@@ -27566,7 +27496,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -27831,10 +27761,8 @@
       <c r="CN47" t="n">
         <v>0</v>
       </c>
-      <c r="CO47" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO47" t="n">
+        <v>0</v>
       </c>
       <c r="CP47" t="n">
         <v>0</v>
@@ -28083,7 +28011,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -28348,10 +28276,8 @@
       <c r="CN48" t="n">
         <v>0</v>
       </c>
-      <c r="CO48" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO48" t="n">
+        <v>0</v>
       </c>
       <c r="CP48" t="n">
         <v>0</v>
@@ -28600,7 +28526,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -28865,10 +28791,8 @@
       <c r="CN49" t="n">
         <v>0</v>
       </c>
-      <c r="CO49" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO49" t="n">
+        <v>0</v>
       </c>
       <c r="CP49" t="n">
         <v>0</v>
@@ -29117,7 +29041,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -29382,10 +29306,8 @@
       <c r="CN50" t="n">
         <v>0</v>
       </c>
-      <c r="CO50" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO50" t="n">
+        <v>0</v>
       </c>
       <c r="CP50" t="n">
         <v>0</v>
@@ -29634,7 +29556,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -29899,10 +29821,8 @@
       <c r="CN51" t="n">
         <v>0</v>
       </c>
-      <c r="CO51" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO51" t="n">
+        <v>0</v>
       </c>
       <c r="CP51" t="n">
         <v>0</v>
@@ -30151,7 +30071,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -30416,10 +30336,8 @@
       <c r="CN52" t="n">
         <v>0</v>
       </c>
-      <c r="CO52" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO52" t="n">
+        <v>0</v>
       </c>
       <c r="CP52" t="n">
         <v>0</v>
@@ -30668,7 +30586,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -30933,10 +30851,8 @@
       <c r="CN53" t="n">
         <v>0</v>
       </c>
-      <c r="CO53" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO53" t="n">
+        <v>0</v>
       </c>
       <c r="CP53" t="n">
         <v>0</v>
@@ -31185,7 +31101,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -31450,10 +31366,8 @@
       <c r="CN54" t="n">
         <v>0</v>
       </c>
-      <c r="CO54" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO54" t="n">
+        <v>0</v>
       </c>
       <c r="CP54" t="n">
         <v>0</v>
@@ -31702,7 +31616,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -31967,10 +31881,8 @@
       <c r="CN55" t="n">
         <v>0</v>
       </c>
-      <c r="CO55" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO55" t="n">
+        <v>0</v>
       </c>
       <c r="CP55" t="n">
         <v>0</v>
@@ -32219,7 +32131,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -32484,10 +32396,8 @@
       <c r="CN56" t="n">
         <v>0</v>
       </c>
-      <c r="CO56" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO56" t="n">
+        <v>0</v>
       </c>
       <c r="CP56" t="n">
         <v>0</v>
@@ -32736,7 +32646,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -33001,10 +32911,8 @@
       <c r="CN57" t="n">
         <v>0</v>
       </c>
-      <c r="CO57" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO57" t="n">
+        <v>0</v>
       </c>
       <c r="CP57" t="n">
         <v>0</v>
@@ -33253,7 +33161,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -33518,10 +33426,8 @@
       <c r="CN58" t="n">
         <v>0</v>
       </c>
-      <c r="CO58" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO58" t="n">
+        <v>0</v>
       </c>
       <c r="CP58" t="n">
         <v>0</v>
@@ -33770,7 +33676,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -34035,10 +33941,8 @@
       <c r="CN59" t="n">
         <v>0</v>
       </c>
-      <c r="CO59" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO59" t="n">
+        <v>0</v>
       </c>
       <c r="CP59" t="n">
         <v>0</v>
@@ -34287,7 +34191,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -34552,10 +34456,8 @@
       <c r="CN60" t="n">
         <v>0</v>
       </c>
-      <c r="CO60" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO60" t="n">
+        <v>0</v>
       </c>
       <c r="CP60" t="n">
         <v>0</v>
@@ -34804,7 +34706,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -35069,10 +34971,8 @@
       <c r="CN61" t="n">
         <v>0</v>
       </c>
-      <c r="CO61" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO61" t="n">
+        <v>0</v>
       </c>
       <c r="CP61" t="n">
         <v>0</v>
@@ -35321,7 +35221,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -35586,10 +35486,8 @@
       <c r="CN62" t="n">
         <v>0</v>
       </c>
-      <c r="CO62" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO62" t="n">
+        <v>0</v>
       </c>
       <c r="CP62" t="n">
         <v>0</v>
@@ -35838,7 +35736,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -36103,10 +36001,8 @@
       <c r="CN63" t="n">
         <v>0</v>
       </c>
-      <c r="CO63" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO63" t="n">
+        <v>0</v>
       </c>
       <c r="CP63" t="n">
         <v>0</v>
@@ -36355,7 +36251,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -36620,10 +36516,8 @@
       <c r="CN64" t="n">
         <v>0</v>
       </c>
-      <c r="CO64" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO64" t="n">
+        <v>0</v>
       </c>
       <c r="CP64" t="n">
         <v>0</v>
@@ -36872,7 +36766,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -37137,10 +37031,8 @@
       <c r="CN65" t="n">
         <v>0</v>
       </c>
-      <c r="CO65" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO65" t="n">
+        <v>0</v>
       </c>
       <c r="CP65" t="n">
         <v>0</v>
@@ -37389,7 +37281,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -37654,10 +37546,8 @@
       <c r="CN66" t="n">
         <v>0</v>
       </c>
-      <c r="CO66" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO66" t="n">
+        <v>0</v>
       </c>
       <c r="CP66" t="n">
         <v>0</v>
@@ -37906,7 +37796,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -38171,10 +38061,8 @@
       <c r="CN67" t="n">
         <v>0</v>
       </c>
-      <c r="CO67" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO67" t="n">
+        <v>0</v>
       </c>
       <c r="CP67" t="n">
         <v>0</v>
@@ -38423,7 +38311,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -38688,10 +38576,8 @@
       <c r="CN68" t="n">
         <v>0</v>
       </c>
-      <c r="CO68" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO68" t="n">
+        <v>0</v>
       </c>
       <c r="CP68" t="n">
         <v>0</v>
@@ -38940,7 +38826,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -39205,10 +39091,8 @@
       <c r="CN69" t="n">
         <v>0</v>
       </c>
-      <c r="CO69" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO69" t="n">
+        <v>0</v>
       </c>
       <c r="CP69" t="n">
         <v>0</v>
@@ -39457,7 +39341,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -39722,10 +39606,8 @@
       <c r="CN70" t="n">
         <v>0</v>
       </c>
-      <c r="CO70" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO70" t="n">
+        <v>0</v>
       </c>
       <c r="CP70" t="n">
         <v>0</v>
@@ -39974,7 +39856,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -40239,10 +40121,8 @@
       <c r="CN71" t="n">
         <v>0</v>
       </c>
-      <c r="CO71" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO71" t="n">
+        <v>0</v>
       </c>
       <c r="CP71" t="n">
         <v>0</v>
@@ -40491,7 +40371,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -40756,10 +40636,8 @@
       <c r="CN72" t="n">
         <v>0</v>
       </c>
-      <c r="CO72" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO72" t="n">
+        <v>0</v>
       </c>
       <c r="CP72" t="n">
         <v>0</v>
@@ -41008,7 +40886,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -41273,10 +41151,8 @@
       <c r="CN73" t="n">
         <v>0</v>
       </c>
-      <c r="CO73" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO73" t="n">
+        <v>0</v>
       </c>
       <c r="CP73" t="n">
         <v>0</v>
@@ -41525,7 +41401,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -41790,10 +41666,8 @@
       <c r="CN74" t="n">
         <v>0</v>
       </c>
-      <c r="CO74" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO74" t="n">
+        <v>0</v>
       </c>
       <c r="CP74" t="n">
         <v>0</v>
@@ -42042,7 +41916,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -42307,10 +42181,8 @@
       <c r="CN75" t="n">
         <v>0</v>
       </c>
-      <c r="CO75" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO75" t="n">
+        <v>0</v>
       </c>
       <c r="CP75" t="n">
         <v>0</v>
@@ -42559,7 +42431,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -42824,10 +42696,8 @@
       <c r="CN76" t="n">
         <v>0</v>
       </c>
-      <c r="CO76" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO76" t="n">
+        <v>0</v>
       </c>
       <c r="CP76" t="n">
         <v>0</v>
@@ -43076,7 +42946,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -43341,10 +43211,8 @@
       <c r="CN77" t="n">
         <v>0</v>
       </c>
-      <c r="CO77" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO77" t="n">
+        <v>0</v>
       </c>
       <c r="CP77" t="n">
         <v>0</v>
@@ -43593,7 +43461,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -43858,10 +43726,8 @@
       <c r="CN78" t="n">
         <v>0</v>
       </c>
-      <c r="CO78" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO78" t="n">
+        <v>0</v>
       </c>
       <c r="CP78" t="n">
         <v>0</v>
@@ -44110,7 +43976,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -44375,10 +44241,8 @@
       <c r="CN79" t="n">
         <v>0</v>
       </c>
-      <c r="CO79" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO79" t="n">
+        <v>0</v>
       </c>
       <c r="CP79" t="n">
         <v>0</v>
@@ -44627,7 +44491,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -44892,10 +44756,8 @@
       <c r="CN80" t="n">
         <v>0</v>
       </c>
-      <c r="CO80" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO80" t="n">
+        <v>0</v>
       </c>
       <c r="CP80" t="n">
         <v>0</v>
@@ -45144,7 +45006,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -45409,10 +45271,8 @@
       <c r="CN81" t="n">
         <v>0</v>
       </c>
-      <c r="CO81" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO81" t="n">
+        <v>0</v>
       </c>
       <c r="CP81" t="n">
         <v>0</v>
@@ -45661,7 +45521,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -45926,10 +45786,8 @@
       <c r="CN82" t="n">
         <v>0</v>
       </c>
-      <c r="CO82" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO82" t="n">
+        <v>0</v>
       </c>
       <c r="CP82" t="n">
         <v>0</v>
@@ -46178,7 +46036,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -46443,10 +46301,8 @@
       <c r="CN83" t="n">
         <v>0</v>
       </c>
-      <c r="CO83" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO83" t="n">
+        <v>0</v>
       </c>
       <c r="CP83" t="n">
         <v>0</v>
@@ -46695,7 +46551,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -46960,10 +46816,8 @@
       <c r="CN84" t="n">
         <v>0</v>
       </c>
-      <c r="CO84" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO84" t="n">
+        <v>0</v>
       </c>
       <c r="CP84" t="n">
         <v>0</v>
@@ -47212,7 +47066,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -47477,10 +47331,8 @@
       <c r="CN85" t="n">
         <v>0</v>
       </c>
-      <c r="CO85" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO85" t="n">
+        <v>0</v>
       </c>
       <c r="CP85" t="n">
         <v>0</v>
@@ -47729,7 +47581,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -47994,10 +47846,8 @@
       <c r="CN86" t="n">
         <v>0</v>
       </c>
-      <c r="CO86" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO86" t="n">
+        <v>0</v>
       </c>
       <c r="CP86" t="n">
         <v>0</v>
@@ -48246,7 +48096,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -48511,10 +48361,8 @@
       <c r="CN87" t="n">
         <v>0</v>
       </c>
-      <c r="CO87" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO87" t="n">
+        <v>0</v>
       </c>
       <c r="CP87" t="n">
         <v>0</v>
@@ -48763,7 +48611,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -49028,10 +48876,8 @@
       <c r="CN88" t="n">
         <v>0</v>
       </c>
-      <c r="CO88" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO88" t="n">
+        <v>0</v>
       </c>
       <c r="CP88" t="n">
         <v>0</v>
@@ -49280,7 +49126,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -49545,10 +49391,8 @@
       <c r="CN89" t="n">
         <v>0</v>
       </c>
-      <c r="CO89" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO89" t="n">
+        <v>0</v>
       </c>
       <c r="CP89" t="n">
         <v>0</v>
@@ -49797,7 +49641,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -50062,10 +49906,8 @@
       <c r="CN90" t="n">
         <v>0</v>
       </c>
-      <c r="CO90" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO90" t="n">
+        <v>0</v>
       </c>
       <c r="CP90" t="n">
         <v>0</v>
@@ -50314,7 +50156,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -50579,10 +50421,8 @@
       <c r="CN91" t="n">
         <v>0</v>
       </c>
-      <c r="CO91" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO91" t="n">
+        <v>0</v>
       </c>
       <c r="CP91" t="n">
         <v>0</v>
@@ -50831,7 +50671,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -51096,10 +50936,8 @@
       <c r="CN92" t="n">
         <v>0</v>
       </c>
-      <c r="CO92" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO92" t="n">
+        <v>0</v>
       </c>
       <c r="CP92" t="n">
         <v>0</v>
@@ -51348,7 +51186,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -51613,10 +51451,8 @@
       <c r="CN93" t="n">
         <v>0</v>
       </c>
-      <c r="CO93" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO93" t="n">
+        <v>0</v>
       </c>
       <c r="CP93" t="n">
         <v>0</v>
@@ -51865,7 +51701,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -52130,10 +51966,8 @@
       <c r="CN94" t="n">
         <v>0</v>
       </c>
-      <c r="CO94" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO94" t="n">
+        <v>0</v>
       </c>
       <c r="CP94" t="n">
         <v>0</v>
@@ -52382,7 +52216,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -52647,10 +52481,8 @@
       <c r="CN95" t="n">
         <v>0</v>
       </c>
-      <c r="CO95" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO95" t="n">
+        <v>0</v>
       </c>
       <c r="CP95" t="n">
         <v>0</v>
@@ -52899,7 +52731,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -53164,10 +52996,8 @@
       <c r="CN96" t="n">
         <v>0</v>
       </c>
-      <c r="CO96" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO96" t="n">
+        <v>0</v>
       </c>
       <c r="CP96" t="n">
         <v>0</v>
@@ -53416,7 +53246,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -53681,10 +53511,8 @@
       <c r="CN97" t="n">
         <v>0</v>
       </c>
-      <c r="CO97" t="inlineStr">
-        <is>
-          <t>VALUES</t>
-        </is>
+      <c r="CO97" t="n">
+        <v>0</v>
       </c>
       <c r="CP97" t="n">
         <v>0</v>
@@ -54166,7 +53994,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -54238,7 +54066,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -54310,7 +54138,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -54382,7 +54210,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>250080</v>
+        <v>227799</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>

</xml_diff>